<commit_message>
compaleted payment integration flow
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -484,7 +484,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-12-26T04:20:37.225Z</v>
+        <v>2025-12-26T20:47:32.579Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -493,7 +493,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-java-developer-simho-hr-services-chennai-1-to-3-years-261225003742</v>
+        <v>https://www.naukri.com/job-listings-full-stack-java-developer-forward-eye-technologies-visakhapatnam-1-to-4-years-261225917104</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -502,10 +502,10 @@
         <v>Yes</v>
       </c>
       <c r="G2" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H2" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I2" t="str">
         <v>3/undefined</v>
@@ -517,22 +517,22 @@
         <v>Direct Apply</v>
       </c>
       <c r="L2" t="str">
-        <v>Java Developer</v>
+        <v>Full Stack Java Developer</v>
       </c>
       <c r="M2" t="str">
-        <v>Simho Hr Services</v>
+        <v>Forward Eye Technologies</v>
       </c>
       <c r="N2" t="str">
-        <v>1 - 3 years</v>
+        <v>1 - 4 years</v>
       </c>
       <c r="O2" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P2" t="str">
-        <v>Chennai</v>
+        <v>Visakhapatnam</v>
       </c>
       <c r="Q2" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R2" t="str">
         <v>1</v>
@@ -541,13 +541,13 @@
         <v>100+</v>
       </c>
       <c r="T2" t="str">
-        <v>Java, Java Spring Boot, Angular</v>
+        <v>sql, react.js, java, javascript, spring boot, continuous integration, kubernetes, redux, web services, ci/cd, docker, git, postgresql, gcp, devops, mysql, typescript, mongodb, agile methodology, rest, oracle, microsoft azure, nosql, aws, sdlc</v>
       </c>
       <c r="U2" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="V2" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W2" t="str">
         <v>Full Time, Permanent</v>
@@ -555,13 +555,16 @@
       <c r="X2" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Y2" t="str">
+        <v>4.9</v>
+      </c>
       <c r="Z2" t="str">
-        <v>Engineering degree or equivalent with 1-3 years experience in web applications using Java framework | Develop and maintain web applications using Java Spring Boot and Angular</v>
+        <v>Proficient in Java, Spring Boot, React.js, and SQL with strong experience in Agile methodologies | Develop and maintain scalable web applications, collaborate with cross-functional teams, and ensure code quality</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-12-26T04:20:42.122Z</v>
+        <v>2025-12-26T20:47:37.307Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -570,7 +573,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-devloper-it-fullstack-ssc-welspun-transformation-services-limited-hyderabad-3-to-5-years-251225009474</v>
+        <v>https://www.naukri.com/job-listings-full-stack-java-developer-forward-eye-technologies-mumbai-1-to-4-years-261225917074</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -594,28 +597,31 @@
         <v>Direct Apply</v>
       </c>
       <c r="L3" t="str">
-        <v>Devloper_IT_Fullstack_SSC</v>
+        <v>Full Stack Java Developer</v>
       </c>
       <c r="M3" t="str">
-        <v>Welspun Transformation Services Limited</v>
+        <v>Forward Eye Technologies</v>
       </c>
       <c r="N3" t="str">
-        <v>3 - 5 years</v>
+        <v>1 - 4 years</v>
       </c>
       <c r="O3" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P3" t="str">
-        <v>Hyderabad</v>
+        <v>Mumbai</v>
       </c>
       <c r="Q3" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R3" t="str">
+        <v>1</v>
+      </c>
+      <c r="S3" t="str">
         <v>100+</v>
       </c>
       <c r="T3" t="str">
-        <v>fullstack development, stack, css, hibernate, ajax, jquery, microservices, spring, react.js, java, git, json, html, mysql, data structures, mongodb, rest, software development, javascript, angular, spring boot, node.js, full stack, front, angularjs</v>
+        <v>sql, react.js, java, javascript, spring boot, continuous integration, kubernetes, redux, web services, ci/cd, docker, git, postgresql, gcp, devops, mysql, typescript, mongodb, agile methodology, rest, oracle, microsoft azure, nosql, aws, sdlc</v>
       </c>
       <c r="U3" t="str">
         <v>Full Stack Developer</v>
@@ -630,15 +636,15 @@
         <v>Software Development</v>
       </c>
       <c r="Y3" t="str">
-        <v>3.6</v>
+        <v>4.9</v>
       </c>
       <c r="Z3" t="str">
-        <v>Experience in Java, Spring Boot, and front-end technologies | Manage server-side logic and integrate front-end elements</v>
+        <v>Proficient in Java, Spring Boot, React.js, and SQL with strong experience in web application development | Develop and maintain scalable web applications, collaborate with cross-functional teams, and ensure code quality</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-12-26T04:21:15.568Z</v>
+        <v>2025-12-26T20:47:51.292Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -647,7 +653,7 @@
         <v>3/20</v>
       </c>
       <c r="D4" t="str">
-        <v>https://www.naukri.com/job-listings-developer-it-reactnativefullstack-ssc-welspun-transformation-services-limited-hyderabad-3-to-5-years-251225009835</v>
+        <v>https://www.naukri.com/job-listings-full-stack-developer-plsql-java-oracle-india-pvt-ltd-mumbai-3-to-8-years-261225908749</v>
       </c>
       <c r="E4" t="str">
         <v>Yes</v>
@@ -668,31 +674,34 @@
         <v>Good Match</v>
       </c>
       <c r="K4" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L4" t="str">
-        <v>Developer_IT_ReactNativeFullstack_SSC</v>
+        <v>Full Stack Developer-PLSQL /Java</v>
       </c>
       <c r="M4" t="str">
-        <v>Welspun Transformation Services Limited</v>
+        <v>Oracle</v>
       </c>
       <c r="N4" t="str">
-        <v>3 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="O4" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P4" t="str">
-        <v>Hyderabad</v>
+        <v>Mumbai</v>
       </c>
       <c r="Q4" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R4" t="str">
-        <v>50+</v>
+        <v>1</v>
+      </c>
+      <c r="S4" t="str">
+        <v>18</v>
       </c>
       <c r="T4" t="str">
-        <v>redux, information technology, jquery, sql, spring, java, git, asp.net, web api, html, mvc, architectural design, c#, python, asp.net mvc, software development, entity framework, react native, javascript, sql server, angular, spring boot, full stack, .net, php</v>
+        <v>PLSQL, prototyping, full stack developer, react, jmeter, ui ux, sql, microservices, java, git, ui, jboss, waterfall, shell scripting, jira, rest, ux, oracle, maven, ai, weblogic, gradle, angular, nlp, full stack, agile, sdlc, soap</v>
       </c>
       <c r="U4" t="str">
         <v>Full Stack Developer</v>
@@ -707,15 +716,15 @@
         <v>Software Development</v>
       </c>
       <c r="Y4" t="str">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="Z4" t="str">
-        <v>Experience with React Native and Redux; strong skills in architectural design | Develop and implement user interface components; ensure application responsiveness; collaborate with graphic designers</v>
+        <v>Recent graduate or postgraduate with 3-9 years of experience; strong Oracle tech skills including PL/SQL, SQL, and Java; exposure to BFSI domain | Develop and customize Oracle applications; assist in testing and deployment; prepare technical documentation</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-12-26T04:21:50.762Z</v>
+        <v>2025-12-26T20:47:56.092Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -724,7 +733,7 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-lead-analyst-java-fullstack-developer-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-6-years-261225904555</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-senior-developer-infosys-limited-coimbatore-3-to-5-years-220925928001</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
@@ -733,43 +742,46 @@
         <v>Yes</v>
       </c>
       <c r="G5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H5" t="str">
         <v>Yes</v>
       </c>
       <c r="I5" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J5" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K5" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L5" t="str">
-        <v>Lead analyst-Java Fullstack Developer</v>
+        <v>Java Full Stack Senior Developer</v>
       </c>
       <c r="M5" t="str">
-        <v>CGI</v>
+        <v>Infosys</v>
       </c>
       <c r="N5" t="str">
-        <v>3 - 6 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="O5" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P5" t="str">
-        <v>Bengaluru</v>
+        <v>Coimbatore</v>
       </c>
       <c r="Q5" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R5" t="str">
+        <v>1</v>
+      </c>
+      <c r="S5" t="str">
         <v>Less than 10</v>
       </c>
       <c r="T5" t="str">
-        <v>java, web security, rest, github, restful, oracle, software development, unit testing, hibernate, code quality, sql, angular, spring boot, scripting, apis, devops, linux, jenkins, debugging, scrum, distributed systems, gitlab, multithreading</v>
+        <v>java development, microservices, spring, apache camel, spring boot, activemq, project management, messaging framework, api integration, rabbitmq, jquery, react.js, java, apache, design patterns, kafka, full stack, api, web application development, project estimation</v>
       </c>
       <c r="U5" t="str">
         <v>Full Stack Developer</v>
@@ -784,15 +796,15 @@
         <v>Software Development</v>
       </c>
       <c r="Y5" t="str">
-        <v>4.0</v>
+        <v>3.5</v>
       </c>
       <c r="Z5" t="str">
-        <v>3-6 years of experience in Java (JDK 17), Spring Boot, and Oracle databases; strong problem-solving skills | Develop and maintain backend applications, manage deployments, collaborate with teams, and conduct unit testing</v>
+        <v>Bachelor of Engineering with high proficiency in Java Development and experience in Spring Boot, Microservices, and e-commerce web application development | Design, develop, validate, and support technology solutions; gather client requirements and translate them into system specifications; contribute to project estimations and coding across the technical stack</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-12-26T04:22:04.661Z</v>
+        <v>2025-12-26T20:48:02.202Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -801,13 +813,13 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-java-developer-jsp-struts-indihire-consultants-chennai-bengaluru-mumbai-all-areas-3-to-8-years-261225004268</v>
+        <v>https://www.naukri.com/job-listings-java-developer-virtusa-consulting-services-pvt-ltd-hyderabad-2-to-7-years-261225920890</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
       </c>
       <c r="F6" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G6" t="str">
         <v>Yes</v>
@@ -816,46 +828,43 @@
         <v>Yes</v>
       </c>
       <c r="I6" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K6" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L6" t="str">
-        <v>Java Developer + JSP + Struts</v>
+        <v>Java Developer</v>
       </c>
       <c r="M6" t="str">
-        <v>Techwise Digital</v>
+        <v>Virtusa</v>
       </c>
       <c r="N6" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="O6" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P6" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Hyderabad</v>
       </c>
       <c r="Q6" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R6" t="str">
-        <v>1</v>
-      </c>
-      <c r="S6" t="str">
-        <v>23</v>
+        <v>50+</v>
       </c>
       <c r="T6" t="str">
-        <v>JSP, Struts, JSP Servlets, Struts Framework</v>
+        <v>java developer, css, nginx, maven, build tools, weblogic, caching, javascript, redis, sql server, sql, gradle, qa, spring boot, database management, java, jboss, mission critical systems, application security, full stack, software solutions, mvc</v>
       </c>
       <c r="U6" t="str">
-        <v>Back End Developer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V6" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Banking</v>
       </c>
       <c r="W6" t="str">
         <v>Full Time, Permanent</v>
@@ -863,13 +872,16 @@
       <c r="X6" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Y6" t="str">
+        <v>3.7</v>
+      </c>
       <c r="Z6" t="str">
-        <v>Experienced in JSP and Struts with strong understanding of server-side MVC architecture | Work on legacy JSP and Struts-based enterprise application, integrate with backend services, and handle form validations</v>
+        <v>4-6 years of experience in .NET Core development, strong skills in MS SQL Server and ASP.NET Core MVC | Design, develop, and maintain high-performance applications; manage databases and ensure code quality</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-12-26T04:22:09.560Z</v>
+        <v>2025-12-26T20:48:16.349Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -878,7 +890,7 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-java-developer-bangalore-pan-india-infosys-infosys-hyderabad-pune-bengaluru-3-to-5-years-171025021070</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-infosys-limited-hubli-3-to-5-years-290925926272</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
@@ -887,22 +899,22 @@
         <v>Yes</v>
       </c>
       <c r="G7" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H7" t="str">
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K7" t="str">
-        <v>No Apply Button</v>
+        <v>External Apply</v>
       </c>
       <c r="L7" t="str">
-        <v>Java Developer- Bangalore (Pan India Infosys)</v>
+        <v>Java Full Stack Developer</v>
       </c>
       <c r="M7" t="str">
         <v>Infosys</v>
@@ -914,22 +926,22 @@
         <v>Not Disclosed</v>
       </c>
       <c r="P7" t="str">
-        <v>Pune</v>
+        <v>Hubli</v>
       </c>
       <c r="Q7" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R7" t="str">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="S7" t="str">
-        <v>50+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T7" t="str">
-        <v>Java, Spring Boot, Hibernate, Spring Mvc, Microservices</v>
+        <v>spring boot, angular, react.js, java, reactive programming, schema, rest, junit, software testing, maven, manual testing, hibernate, javascript, application development, spring, ui, java code, full stack, architectural patterns, servlets, troubleshooting, aws</v>
       </c>
       <c r="U7" t="str">
-        <v>Software Development - Other</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V7" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -944,12 +956,12 @@
         <v>3.5</v>
       </c>
       <c r="Z7" t="str">
-        <v>Java developer with 3+ years of experience and a degree in BE/B.Tech/MCA/M.Tech/MSc./MS | Aid consulting team in project phases, create requirement specifications, and support solution configuration</v>
+        <v>MCA, MTech, or Bachelor of Engineering with 3+ years of experience in Java and Angular or React or AWS | Analyze user requirements, design and maintain Java codes, troubleshoot development issues, and implement automated testing</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-12-26T04:22:14.437Z</v>
+        <v>2025-12-26T20:48:21.450Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -958,7 +970,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-app-dev-support-engineer-i-conduent-business-services-india-llp-bengaluru-1-to-5-years-261225904533</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-6-years-261225920170</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -982,13 +994,13 @@
         <v>Direct Apply</v>
       </c>
       <c r="L8" t="str">
-        <v>App Dev &amp; Support Engineer I</v>
+        <v>Java full stack Developer</v>
       </c>
       <c r="M8" t="str">
-        <v>Conduent</v>
+        <v>CGI</v>
       </c>
       <c r="N8" t="str">
-        <v>1 - 5 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="O8" t="str">
         <v>Not Disclosed</v>
@@ -997,36 +1009,36 @@
         <v>Bengaluru</v>
       </c>
       <c r="Q8" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R8" t="str">
-        <v>15</v>
+        <v>50+</v>
       </c>
       <c r="T8" t="str">
-        <v>css, rest, oracle, apache ant, rest api, maven, version control, weblogic, hibernate, analytical skills, javascript, sql, microservices, angular, spring boot, java, apache, xml, web technologies, design, servlets, troubleshooting, html</v>
+        <v>Java, rest, restful, streaming data, system programming, full stack developer, microservices, angular, automation, product development, full stack, agile methodologies, scrum, software engineering, agile, aws, programming, financial markets</v>
       </c>
       <c r="U8" t="str">
-        <v>Database Administrator</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V8" t="str">
-        <v>BPM / BPO</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W8" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X8" t="str">
-        <v>DBA / Data warehousing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y8" t="str">
-        <v>3.4</v>
+        <v>4.0</v>
       </c>
       <c r="Z8" t="str">
-        <v>. Must have experience in working with version control systems like RTC | Loves to learn and develop new skills continuously . Must have strong troubleshooting skills</v>
+        <v>Proficiency in Java, Angular, Microservices, and AWS; experience in financial markets and system programming | Drive technical discussions, maintain CI/CD pipelines, and contribute to software design and development</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-12-26T04:22:28.573Z</v>
+        <v>2025-12-26T20:48:35.190Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1035,13 +1047,13 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-data-scientist-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-8-years-261225904548</v>
+        <v>https://www.naukri.com/job-listings-software-engineer-ge-renewable-energy-technologies-private-limited-bengaluru-2-to-5-years-261225926791</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
       </c>
       <c r="F9" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G9" t="str">
         <v>Yes</v>
@@ -1050,22 +1062,22 @@
         <v>Yes</v>
       </c>
       <c r="I9" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J9" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K9" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L9" t="str">
-        <v>Data Scientist</v>
+        <v>Software Engineer</v>
       </c>
       <c r="M9" t="str">
-        <v>CGI</v>
+        <v>GE VERNOVA</v>
       </c>
       <c r="N9" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O9" t="str">
         <v>Not Disclosed</v>
@@ -1074,36 +1086,36 @@
         <v>Bengaluru</v>
       </c>
       <c r="Q9" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R9" t="str">
-        <v>14</v>
+        <v>100+</v>
       </c>
       <c r="T9" t="str">
-        <v>data scientist, kubernetes, python, natural language processing, forecasting, nltk, ai, numpy, machine learning, docker, pandas, tensorflow, spacy, git, nlp, data science, spark, business insights, pytorch, mysql, hadoop, big data</v>
+        <v>Software Engineer, Java, Postgresql, Ai, User Experience, Full Stack, Restful, React, Machine Learning, Angular, Sql, Restful Apis, Jenkins, Software Development, Front End, Git, Docker, Mysql, Agile, Postgres, Aws, Oracle, Due Diligence, Kubernetes</v>
       </c>
       <c r="U9" t="str">
-        <v>Full Stack Data Scientist</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V9" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Power</v>
       </c>
       <c r="W9" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X9" t="str">
-        <v>Data Science &amp; Machine Learning</v>
+        <v>Software Development</v>
       </c>
       <c r="Y9" t="str">
-        <v>4.0</v>
+        <v>4.1</v>
       </c>
       <c r="Z9" t="str">
-        <v>Master's degree in Computer Science or Data Science with 3+ years of experience in machine learning and data science roles | Develop and operationalize machine learning models, focusing on NLP sentiment analysis, app recommendations, and sales forecasting | Competitive salary and benefits package</v>
+        <v>Bachelor's degree in Computer Science or STEM with 2-5 years of experience; proficiency in Full Stack .NET (C#) or Java, and modern front-end frameworks like Angular or React | Program and develop software components, maintain code quality, engage in technical discussions, and optimize application performance | Relocation assistance provided</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-12-26T04:22:33.467Z</v>
+        <v>2025-12-26T20:48:49.264Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1112,7 +1124,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-software-test-engineer-onsite-mumbai-baldor-technologies-mumbai-3-to-6-years-241225021650</v>
+        <v>https://www.naukri.com/job-listings-full-stack-software-developer-java-web-technologies-oracle-india-pvt-ltd-bengaluru-3-to-6-years-261225908763</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1133,13 +1145,13 @@
         <v>Good Match</v>
       </c>
       <c r="K10" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L10" t="str">
-        <v>Software Test Engineer- Onsite Mumbai</v>
+        <v>Full Stack Software Developer Java/Web Technologies</v>
       </c>
       <c r="M10" t="str">
-        <v>Baldor Technologies</v>
+        <v>Oracle</v>
       </c>
       <c r="N10" t="str">
         <v>3 - 6 years</v>
@@ -1148,42 +1160,42 @@
         <v>Not Disclosed</v>
       </c>
       <c r="P10" t="str">
-        <v>Mumbai( Marol )</v>
+        <v>Bengaluru</v>
       </c>
       <c r="Q10" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R10" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S10" t="str">
-        <v>100+</v>
+        <v>13</v>
       </c>
       <c r="T10" t="str">
-        <v>Automation Testing, Github Actions, Testrail, Ci/Cd, Zephyr, JIRA, Api Automation, Docker, Rest Assured, Framework Design, API Testing, Javascript, Web Automation Testing, Selenium, Cypress Automation, Web Testing</v>
+        <v>JavaScript, restful, software development, business intelligence, microservices, docker, configuration management, java, git, automation, devops, web technologies, full stack, debugging, software developer</v>
       </c>
       <c r="U10" t="str">
-        <v>Automation Test Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V10" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W10" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X10" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y10" t="str">
-        <v>4.0</v>
+        <v>3.5</v>
       </c>
       <c r="Z10" t="str">
-        <v>Graduate with 3 to 6 years of experience in test automation, especially with Cypress and Playwright | Develop and execute automated test scripts, collaborate with teams to integrate testing into CI/CD, and monitor test coverage</v>
+        <v>Bachelor's or Master's degree in Computer Science; 4+ years of experience in Java, J2EE, and modern web frameworks; strong knowledge of data structures and algorithms | Develop and debug software applications; perform technical design and code development; contribute to DevOps initiatives</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-12-26T04:23:08.868Z</v>
+        <v>2025-12-26T20:48:53.952Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1192,13 +1204,13 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-penetration-tester-application-security-analyst-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-8-years-261225904575</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-sarvaha-pune-3-to-8-years-261225917323</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
       </c>
       <c r="F11" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G11" t="str">
         <v>Yes</v>
@@ -1207,19 +1219,19 @@
         <v>Yes</v>
       </c>
       <c r="I11" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J11" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K11" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L11" t="str">
-        <v>Penetration Tester / Application Security Analyst</v>
+        <v>Java Full stack Developer</v>
       </c>
       <c r="M11" t="str">
-        <v>CGI</v>
+        <v>Sarvaha Systems</v>
       </c>
       <c r="N11" t="str">
         <v>3 - 8 years</v>
@@ -1228,19 +1240,22 @@
         <v>Not Disclosed</v>
       </c>
       <c r="P11" t="str">
-        <v>Bengaluru</v>
+        <v>Pune</v>
       </c>
       <c r="Q11" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R11" t="str">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="S11" t="str">
+        <v>100+</v>
       </c>
       <c r="T11" t="str">
-        <v>application security, python, cloud security, oscp, ceh, security automation, manual testing, vulnerability assessment, cybersecurity, javascript, gdpr, dast, gcp, compliance, powershell, bash, penetration testing, sast, devsecops, aws, sdlc, azure</v>
+        <v>Java, React, Angular, Hibernate, PostgreSQL, Java Full stack Developer, Microservices, Jenkins, Git, Docker, MySQL, MongoDB, Spring boot, Kubernetes</v>
       </c>
       <c r="U11" t="str">
-        <v>Security Testing Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V11" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1249,18 +1264,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X11" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y11" t="str">
-        <v>4.0</v>
+        <v>4.5</v>
       </c>
       <c r="Z11" t="str">
-        <v>3+ years of experience in penetration testing, proficiency in Burp Suite, and scripting knowledge in Python or JavaScript | Conduct manual penetration testing, identify vulnerabilities, and document findings</v>
+        <v>BE/BTech/MTech in CS/IT or MCA with 3+ years of experience in Java and backend services | Design, develop, and maintain scalable applications; collaborate with teams to deliver high-quality solutions | Top-notch remuneration and excellent growth opportunities</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-12-26T04:23:13.949Z</v>
+        <v>2025-12-26T20:49:07.607Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1269,13 +1284,13 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-senior-software-engineer-lead-analyst-security-testing-cgi-information-systems-and-management-consultants-private-limited-chennai-3-to-8-years-261225904569</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-261225918782</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
       </c>
       <c r="F12" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G12" t="str">
         <v>Yes</v>
@@ -1284,22 +1299,22 @@
         <v>Yes</v>
       </c>
       <c r="I12" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J12" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K12" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L12" t="str">
-        <v>Senior Software Engineer/Lead Analyst-Security Testing</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M12" t="str">
-        <v>CGI</v>
+        <v>Accenture</v>
       </c>
       <c r="N12" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O12" t="str">
         <v>Not Disclosed</v>
@@ -1308,16 +1323,16 @@
         <v>Chennai</v>
       </c>
       <c r="Q12" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R12" t="str">
         <v>Less than 10</v>
       </c>
       <c r="T12" t="str">
-        <v>software engineer, risk management, python, cloud security, oscp, penetration testing methodologies, manual testing, javascript, gdpr, dast, security testing, gcp, compliance, powershell, bash, penetration testing, sast, devsecops, aws, sdlc, azure</v>
+        <v>software engineer, application developer, css, version control, business processes, hibernate, javascript, nosql, sql, database management, java, git, web technologies, full stack, software solutions, construction, html, agile, nosql databases</v>
       </c>
       <c r="U12" t="str">
-        <v>Security Testing Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V12" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1326,18 +1341,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X12" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y12" t="str">
-        <v>4.0</v>
+        <v>3.7</v>
       </c>
       <c r="Z12" t="str">
-        <v>Bachelor's degree in computer science or related field with 3+ years of penetration testing experience; proficiency in Burp Suite Pro and cloud security testing | Lead and perform advanced manual penetration testing; manage and mentor junior testers; provide strategic recommendations on risk remediation</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in web technologies and frameworks | Develop custom software solutions, collaborate with stakeholders, and mentor junior team members</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-12-26T04:23:18.788Z</v>
+        <v>2025-12-26T20:49:12.849Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1346,7 +1361,7 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-back-end-developer-moneymul-technologies-noida-2-to-7-years-261225000324</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-261225917853</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
@@ -1367,40 +1382,37 @@
         <v>Good Match</v>
       </c>
       <c r="K13" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L13" t="str">
-        <v>Back End Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M13" t="str">
-        <v>Moneymul Technologies</v>
+        <v>Accenture</v>
       </c>
       <c r="N13" t="str">
-        <v>2 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O13" t="str">
-        <v>5-12 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="P13" t="str">
-        <v>Noida</v>
+        <v>Chennai</v>
       </c>
       <c r="Q13" t="str">
-        <v>Today</v>
+        <v>1 day ago</v>
       </c>
       <c r="R13" t="str">
-        <v>5</v>
-      </c>
-      <c r="S13" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T13" t="str">
-        <v>Postgres Database, Debugging, Node.Js, Backend Development, Api Design And Development, Lld Design, Performance Optimization, Postgresql, Database Design, Code Quality, Code Review, Coding Standards, Rest Api Design, Backend, API, Nosql Databases, High Level Design, Expresjs, Indexing</v>
+        <v>software engineer, software development, full stack development, version control, programming principles, sql, spring boot, database management, java, git, design, full stack, software solutions, debugging, agile, programming</v>
       </c>
       <c r="U13" t="str">
-        <v>Back End Developer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V13" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W13" t="str">
         <v>Full Time, Permanent</v>
@@ -1409,15 +1421,15 @@
         <v>Software Development</v>
       </c>
       <c r="Y13" t="str">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="Z13" t="str">
-        <v>2-7 years of experience in backend development with strong proficiency in JavaScript and Node.js | Build scalable server-side applications, ensure timely delivery of high-quality code, and take ownership of modules | Comprehensive health insurance coverage and professional development opportunities</v>
+        <v>Minimum 5 years experience in Java Standard Edition; proficiency in object-oriented programming; familiarity with Agile methodologies | Develop custom software solutions; collaborate with cross-functional teams; mentor junior team members</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-12-26T04:23:56.245Z</v>
+        <v>2025-12-26T20:49:17.694Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1426,13 +1438,13 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-operations-engineer-tata-autocomp-chennai-3-to-7-years-251225012845</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225918403</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
       </c>
       <c r="F14" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G14" t="str">
         <v>Yes</v>
@@ -1441,63 +1453,60 @@
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K14" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L14" t="str">
-        <v>Operations Engineer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M14" t="str">
-        <v>Tata AutoComp</v>
+        <v>Accenture</v>
       </c>
       <c r="N14" t="str">
-        <v>3 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O14" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P14" t="str">
-        <v>Chennai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="Q14" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R14" t="str">
-        <v>1</v>
-      </c>
-      <c r="S14" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T14" t="str">
-        <v>python, Service Request, Incident Management, Escalation Management, CICD, AWS, Resolution</v>
+        <v>software engineer, restful, software development, web services, version control, react, amazon web services, microservices, spring boot, database management, java, git, postgresql, api design, full stack, software solutions, mysql, agile, aws</v>
       </c>
       <c r="U14" t="str">
-        <v>Other</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V14" t="str">
-        <v>Auto Components</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W14" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X14" t="str">
-        <v>Other</v>
+        <v>Software Development</v>
       </c>
       <c r="Y14" t="str">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="Z14" t="str">
-        <v>Basic understanding of AWS/Azure, scripting skills in Python/Bash, and strong analytical skills | Handle incidents and service requests, execute and maintain runbooks, and collaborate with teams</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with skills in AWS, Spring Boot, and React.js | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-12-26T04:24:01.118Z</v>
+        <v>2025-12-26T20:49:22.390Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1506,7 +1515,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-developer-xrapido-freeland-park-poole-1-to-3-years-251225010205</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225917923</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1518,43 +1527,40 @@
         <v>Yes</v>
       </c>
       <c r="H15" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I15" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K15" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L15" t="str">
-        <v>Full Stack Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M15" t="str">
-        <v>Xrapido</v>
+        <v>Accenture</v>
       </c>
       <c r="N15" t="str">
-        <v>1 - 3 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O15" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P15" t="str">
-        <v>Freeland Park,Poole</v>
+        <v>Bengaluru</v>
       </c>
       <c r="Q15" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R15" t="str">
-        <v>1</v>
-      </c>
-      <c r="S15" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T15" t="str">
-        <v>python, Node.Js, React.Js, JSON, MongoDB, Rest Api Services</v>
+        <v>software engineer, restful, software development, web services, version control, react, amazon web services, microservices, spring boot, database management, java, git, postgresql, api design, full stack, software solutions, mysql, agile, aws</v>
       </c>
       <c r="U15" t="str">
         <v>Full Stack Developer</v>
@@ -1568,13 +1574,16 @@
       <c r="X15" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Y15" t="str">
+        <v>3.7</v>
+      </c>
       <c r="Z15" t="str">
-        <v>Fluent in React and Python with strong skills in data scraping and transformation | Build and maintain data scrapers, write rule-based logic, and manage APIs for product data</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development; proficiency in Java, React.js, Spring Boot, and AWS | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-12-26T04:24:05.975Z</v>
+        <v>2025-12-26T20:49:27.122Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1583,13 +1592,13 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-php-and-laravel-developer-indus-health-plus-pune-3-to-5-years-280525018040</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225918695</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
       </c>
       <c r="F16" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G16" t="str">
         <v>Yes</v>
@@ -1598,63 +1607,60 @@
         <v>Yes</v>
       </c>
       <c r="I16" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J16" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K16" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L16" t="str">
-        <v>PHP and Laravel Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M16" t="str">
-        <v>Indus Health Plus</v>
+        <v>Accenture</v>
       </c>
       <c r="N16" t="str">
-        <v>3 - 5 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O16" t="str">
-        <v>2.5-4.5 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="P16" t="str">
-        <v>Pune</v>
+        <v>Bengaluru</v>
       </c>
       <c r="Q16" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R16" t="str">
-        <v>1</v>
-      </c>
-      <c r="S16" t="str">
-        <v>29</v>
+        <v>Less than 10</v>
       </c>
       <c r="T16" t="str">
-        <v>Website Optimization, Ecommerce Development, Ecommerce Domain, Apache, Laravel, Nginx, Payment Gateway Integration, Php Laravel, Payment Gateways, MySQL</v>
+        <v>software engineer, api development, restful, web services, full stack development, version control, react, amazon web services, sql, microservices, spring boot, database management, java, git, full stack, software solutions, agile, aws, architecture</v>
       </c>
       <c r="U16" t="str">
-        <v>IT Support - Other</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V16" t="str">
-        <v>Medical Services / Hospital</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W16" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X16" t="str">
-        <v>IT Support</v>
+        <v>Software Development</v>
       </c>
       <c r="Y16" t="str">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="Z16" t="str">
-        <v>Experience in PHP Laravel and payment gateway integration | Outline day-to-day responsibilities related to ecommerce development and website optimization</v>
+        <v>Minimum 5 years experience in Java Full Stack Development, proficiency in AWS, Spring Boot, and React.js | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-12-26T04:24:11.081Z</v>
+        <v>2025-12-26T20:49:31.843Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1663,13 +1669,13 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-senior-ai-cognitive-developer-cloud-genai-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-8-years-261225904605</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-261225918663</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
       </c>
       <c r="F17" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G17" t="str">
         <v>Yes</v>
@@ -1678,19 +1684,19 @@
         <v>Yes</v>
       </c>
       <c r="I17" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J17" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K17" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L17" t="str">
-        <v>Senior Ai Cognitive Developer (Cloud/GenAI)</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M17" t="str">
-        <v>CGI</v>
+        <v>Accenture</v>
       </c>
       <c r="N17" t="str">
         <v>3 - 8 years</v>
@@ -1699,19 +1705,19 @@
         <v>Not Disclosed</v>
       </c>
       <c r="P17" t="str">
-        <v>Bengaluru</v>
+        <v>Chennai</v>
       </c>
       <c r="Q17" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R17" t="str">
         <v>Less than 10</v>
       </c>
       <c r="T17" t="str">
-        <v>ai, python, generative ai, retail, cloud ai, cloud, ai engineer, java, apis, manufacturing, software engineer, typescript, finance, programming</v>
+        <v>software engineer, application developer, full stack development, version control, business processes, react, sql, spring boot, database management, java, git, design, full stack, software solutions, construction, agile, architecture</v>
       </c>
       <c r="U17" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V17" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1720,18 +1726,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X17" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y17" t="str">
-        <v>4.0</v>
+        <v>3.7</v>
       </c>
       <c r="Z17" t="str">
-        <v>Bachelor's degree in Computer Science or related field with 3+ years of experience; expertise in generative AI and cloud AI | Develop applications using generative AI, work with various business verticals, and utilize programming skills in Java, Python, and TypeScript</v>
+        <v>Minimum 3 years experience in Java Full Stack Development with proficiency in modern frameworks | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-12-26T04:24:16.202Z</v>
+        <v>2025-12-26T20:49:36.510Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1740,16 +1746,16 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-gw-pc-configuration-developer-guidewire-policy-center-configuration-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-8-years-261225904570</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bhubaneswar-2-to-5-years-261225918260</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
       </c>
       <c r="F18" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G18" t="str">
         <v>No</v>
-      </c>
-      <c r="G18" t="str">
-        <v>Yes</v>
       </c>
       <c r="H18" t="str">
         <v>Yes</v>
@@ -1761,34 +1767,34 @@
         <v>Poor Match</v>
       </c>
       <c r="K18" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L18" t="str">
-        <v>GW PC Configuration Developer - Guidewire Policy Center Configuration</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M18" t="str">
-        <v>CGI</v>
+        <v>Accenture</v>
       </c>
       <c r="N18" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="O18" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P18" t="str">
-        <v>Bengaluru</v>
+        <v>Bhubaneswar</v>
       </c>
       <c r="Q18" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R18" t="str">
         <v>Less than 10</v>
       </c>
       <c r="T18" t="str">
-        <v>java, cloud, bc, cloud migration, software engineering, agile, agile methodology</v>
+        <v>software engineer, front end, css, restful, software development, javascript, microservices, back end, software development lifecycle, java, restful apis, git, microservices architecture, full stack, construction, agile, architecture</v>
       </c>
       <c r="U18" t="str">
-        <v>Database Administrator</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V18" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1797,18 +1803,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X18" t="str">
-        <v>DBA / Data warehousing</v>
+        <v>Software Development</v>
       </c>
       <c r="Y18" t="str">
-        <v>4.0</v>
+        <v>3.7</v>
       </c>
       <c r="Z18" t="str">
-        <v>Bachelor's degree in computer science or related field with 5+ years of Guidewire Policy Center configuration experience | Guidewire PC configuration, coding, defect fixing, and Agile methodology delivery</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end and back-end technologies | Develop custom software solutions, collaborate with teams, and mentor junior members</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-12-26T04:24:22.063Z</v>
+        <v>2025-12-26T20:49:41.268Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1817,13 +1823,13 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-technical-business-analysis-engineer-i-conduent-business-services-india-llp-noida-2-to-6-years-261225904553</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-261225918784</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
       </c>
       <c r="F19" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G19" t="str">
         <v>Yes</v>
@@ -1832,60 +1838,60 @@
         <v>Yes</v>
       </c>
       <c r="I19" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J19" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K19" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L19" t="str">
-        <v>Technical Business Analysis Engineer I</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M19" t="str">
-        <v>Conduent</v>
+        <v>Accenture</v>
       </c>
       <c r="N19" t="str">
-        <v>2 - 6 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="O19" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P19" t="str">
-        <v>Noida</v>
+        <v>Bengaluru</v>
       </c>
       <c r="Q19" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R19" t="str">
-        <v>12</v>
+        <v>Less than 10</v>
       </c>
       <c r="T19" t="str">
-        <v>business analysis, project management, css, data analysis, team management, manual testing, business analytics, business development, user stories, market research, sales, sql, marketing, tableau, product management, brd, html, mysql, agile, requirement analysis</v>
+        <v>software engineer, version control, react, amazon web services, user experience, microservices, web development frameworks, spring boot, database management, java, git, data modeling, full stack, software solutions, web development, agile, aws</v>
       </c>
       <c r="U19" t="str">
-        <v>Business Analyst</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V19" t="str">
-        <v>BPM / BPO</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="W19" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="X19" t="str">
-        <v>Business Intelligence &amp; Analytics</v>
+        <v>Software Development</v>
       </c>
       <c r="Y19" t="str">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="Z19" t="str">
-        <v>College or university degree required or equivalent work experience. General Profile | Applies general knowledge of business developed through education or experience. Impact</v>
+        <v>Minimum 3 years experience in Java Full Stack Development, proficiency in React.js, Spring Boot, and AWS | Develop custom software solutions, collaborate with teams to gather requirements, and mentor junior members</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-12-26T04:24:27.024Z</v>
+        <v>2025-12-26T20:49:46.013Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1894,13 +1900,13 @@
         <v>19/20</v>
       </c>
       <c r="D20" t="str">
-        <v>https://www.naukri.com/job-listings-cloud-operations-engineer-devon-software-services-bengaluru-3-to-7-years-261225003821</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-261225917858</v>
       </c>
       <c r="E20" t="str">
         <v>Yes</v>
       </c>
       <c r="F20" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G20" t="str">
         <v>Yes</v>
@@ -1909,43 +1915,40 @@
         <v>Yes</v>
       </c>
       <c r="I20" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J20" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K20" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L20" t="str">
-        <v>Cloud Operations Engineer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M20" t="str">
-        <v>Devon Software Services</v>
+        <v>Accenture</v>
       </c>
       <c r="N20" t="str">
-        <v>3 - 7 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="O20" t="str">
-        <v>8-15 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="P20" t="str">
-        <v>Bengaluru</v>
+        <v>Gurugram</v>
       </c>
       <c r="Q20" t="str">
-        <v>Just now</v>
+        <v>1 day ago</v>
       </c>
       <c r="R20" t="str">
-        <v>1</v>
-      </c>
-      <c r="S20" t="str">
-        <v>50+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T20" t="str">
-        <v>Cloud Operations, Cloudops, Terraform, Cloud Support, AWS, Python</v>
+        <v>software engineer, application developer, restful, ux, version control, business processes, react, sql, web development frameworks, back end, database management, java, git, ui, full stack, debugging, construction, web development, ux design</v>
       </c>
       <c r="U20" t="str">
-        <v>DevOps Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V20" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1954,18 +1957,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X20" t="str">
-        <v>DevOps</v>
+        <v>Software Development</v>
       </c>
       <c r="Y20" t="str">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="Z20" t="str">
-        <v>3 to 7 years of experience in Cloud operations with hands-on experience in Python, NodeJS, or Java | Work on rotational shifts and manage AWS Cloud Services, develop database scripts, and utilize monitoring tools</v>
+        <v>Minimum 3 years experience in Java Full Stack Development; proficiency in React.js; 15 years full-time education | Design, build, and configure applications; participate in testing and debugging; assist in documentation</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-12-26T04:24:31.869Z</v>
+        <v>2025-12-26T20:49:53.162Z</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1974,58 +1977,55 @@
         <v>20/20</v>
       </c>
       <c r="D21" t="str">
-        <v>https://www.naukri.com/job-listings-azure-devops-engineer-intellisource-technologies-pune-3-to-5-years-251225013995</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-3-to-8-years-261225917771</v>
       </c>
       <c r="E21" t="str">
         <v>Yes</v>
       </c>
       <c r="F21" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G21" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H21" t="str">
         <v>Yes</v>
       </c>
       <c r="I21" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J21" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K21" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L21" t="str">
-        <v>Azure DevOps Engineer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="M21" t="str">
-        <v>Intellisource Technologies</v>
+        <v>Accenture</v>
       </c>
       <c r="N21" t="str">
-        <v>3 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="O21" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="P21" t="str">
-        <v>Pune( Baner )</v>
+        <v>Navi Mumbai</v>
       </c>
       <c r="Q21" t="str">
         <v>1 day ago</v>
       </c>
       <c r="R21" t="str">
-        <v>1</v>
-      </c>
-      <c r="S21" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="T21" t="str">
-        <v>Azure Devops, Azure Kubernetes, Artifacts, Linux Administration, Azure Pipelines, Ci Cd Pipeline, Terraform, Powershell, Azure Administration, Yaml</v>
+        <v>software engineer, application developer, cloud services, version control, business processes, sql, web development frameworks, cloud, database management, java, git, business process, full stack, debugging, construction, web development</v>
       </c>
       <c r="U21" t="str">
-        <v>DevOps Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="V21" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -2034,13 +2034,13 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="X21" t="str">
-        <v>DevOps</v>
+        <v>Software Development</v>
       </c>
       <c r="Y21" t="str">
-        <v>2.4</v>
+        <v>3.7</v>
       </c>
       <c r="Z21" t="str">
-        <v>Bachelor's degree in Computer Science or related field; proven experience in Azure DevOps pipeline development; strong knowledge of containerization and orchestration | Design, implement, and maintain CI/CD pipelines; collaborate with teams for seamless integration; automate infrastructure provisioning</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development and 15 years of full-time education | Design, build, and configure applications to meet business requirements, collaborate with teams, and ensure application performance</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add code changes in ui and functions
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -437,54 +437,57 @@
         <v>applyType</v>
       </c>
       <c r="L1" t="str">
+        <v>applicationStatus</v>
+      </c>
+      <c r="M1" t="str">
         <v>jobTitle</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>companyName</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>experienceRequired</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>salary</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>location</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>postedDate</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>openings</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>applicants</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>keySkills</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
         <v>role</v>
       </c>
-      <c r="V1" t="str">
+      <c r="W1" t="str">
         <v>industryType</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>employmentType</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Y1" t="str">
         <v>roleCategory</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>companyRating</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>jobHighlights</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-12-26T20:47:32.579Z</v>
+        <v>2025-12-29T20:38:51.669Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -493,7 +496,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-java-developer-forward-eye-technologies-visakhapatnam-1-to-4-years-261225917104</v>
+        <v>https://www.naukri.com/job-listings-net-developer-wpf-maui-web-api-iot-gvrai-technologies-bengaluru-0-to-3-years-291225028590</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -502,10 +505,10 @@
         <v>Yes</v>
       </c>
       <c r="G2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="H2" t="str">
         <v>No</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Yes</v>
       </c>
       <c r="I2" t="str">
         <v>3/undefined</v>
@@ -517,54 +520,54 @@
         <v>Direct Apply</v>
       </c>
       <c r="L2" t="str">
-        <v>Full Stack Java Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M2" t="str">
-        <v>Forward Eye Technologies</v>
+        <v>.NET Developer (WPF / MAUI / Web API / IoT)</v>
       </c>
       <c r="N2" t="str">
-        <v>1 - 4 years</v>
+        <v>Gvrai Technologies</v>
       </c>
       <c r="O2" t="str">
-        <v>Not Disclosed</v>
+        <v>0 - 3 years</v>
       </c>
       <c r="P2" t="str">
-        <v>Visakhapatnam</v>
+        <v>12-36 Lacs P.A.</v>
       </c>
       <c r="Q2" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R2" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R2" t="str">
-        <v>1</v>
-      </c>
       <c r="S2" t="str">
-        <v>100+</v>
+        <v>1</v>
       </c>
       <c r="T2" t="str">
-        <v>sql, react.js, java, javascript, spring boot, continuous integration, kubernetes, redux, web services, ci/cd, docker, git, postgresql, gcp, devops, mysql, typescript, mongodb, agile methodology, rest, oracle, microsoft azure, nosql, aws, sdlc</v>
+        <v>50+</v>
       </c>
       <c r="U2" t="str">
+        <v>C#, Asp.Net Core, MAUI, WPF, Entity Framework Core, English, .Net Core, C++, Esp32, Sql Server, Microsoft Azure, IoT</v>
+      </c>
+      <c r="V2" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V2" t="str">
+      <c r="W2" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X2" t="str">
+      <c r="Y2" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y2" t="str">
-        <v>4.9</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>Proficient in Java, Spring Boot, React.js, and SQL with strong experience in Agile methodologies | Develop and maintain scalable web applications, collaborate with cross-functional teams, and ensure code quality</v>
+      <c r="AA2" t="str">
+        <v>Expertise in C# and .NET 6+, with hands-on experience in ASP.NET Core Web API and Entity Framework Core | Develop and maintain applications using .NET technologies, including Azure and SQL Server</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-12-26T20:47:37.307Z</v>
+        <v>2025-12-29T20:38:56.594Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -573,7 +576,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-java-developer-forward-eye-technologies-mumbai-1-to-4-years-261225917074</v>
+        <v>https://www.naukri.com/job-listings-net-mvc-developer-rudr-consultancy-services-udaipur-1-to-3-years-291225907594</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -582,69 +585,69 @@
         <v>Yes</v>
       </c>
       <c r="G3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I3" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J3" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K3" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L3" t="str">
-        <v>Full Stack Java Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M3" t="str">
-        <v>Forward Eye Technologies</v>
+        <v>.Net Mvc Developer</v>
       </c>
       <c r="N3" t="str">
-        <v>1 - 4 years</v>
+        <v>Leading Client</v>
       </c>
       <c r="O3" t="str">
+        <v>1 - 3 years</v>
+      </c>
+      <c r="P3" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P3" t="str">
-        <v>Mumbai</v>
-      </c>
       <c r="Q3" t="str">
+        <v>Udaipur</v>
+      </c>
+      <c r="R3" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R3" t="str">
-        <v>1</v>
-      </c>
       <c r="S3" t="str">
-        <v>100+</v>
+        <v>1</v>
       </c>
       <c r="T3" t="str">
-        <v>sql, react.js, java, javascript, spring boot, continuous integration, kubernetes, redux, web services, ci/cd, docker, git, postgresql, gcp, devops, mysql, typescript, mongodb, agile methodology, rest, oracle, microsoft azure, nosql, aws, sdlc</v>
+        <v>42</v>
       </c>
       <c r="U3" t="str">
+        <v>sql, asp.net, mvc, entity framework, .net core, css, web services, ado.net, bootstrap, ajax, jquery, java, oops, json, html, web api, wcf, c#, mvc framework, asp.net mvc, mvc architecture, mvc implementation, sql server, javascript, angular, linq, .net, angularjs, asp</v>
+      </c>
+      <c r="V3" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V3" t="str">
+      <c r="W3" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y3" t="str">
-        <v>4.9</v>
-      </c>
-      <c r="Z3" t="str">
-        <v>Proficient in Java, Spring Boot, React.js, and SQL with strong experience in web application development | Develop and maintain scalable web applications, collaborate with cross-functional teams, and ensure code quality</v>
+      <c r="AA3" t="str">
+        <v>1-3 years experience in .NET, MVC, ASP, Entity Frameworks, C#; BTech, BCA, or MCA degree | Develop software solutions using .NET infrastructure, reformulate existing code, and deliver solutions for large-scale enterprises | Salary is best in the industry</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-12-26T20:47:51.292Z</v>
+        <v>2025-12-29T20:39:02.351Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -653,7 +656,7 @@
         <v>3/20</v>
       </c>
       <c r="D4" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-developer-plsql-java-oracle-india-pvt-ltd-mumbai-3-to-8-years-261225908749</v>
+        <v>https://www.naukri.com/job-listings-net-mvc-developer-rudr-consultancy-services-udaipur-jaipur-1-to-5-years-291225916612</v>
       </c>
       <c r="E4" t="str">
         <v>Yes</v>
@@ -662,69 +665,66 @@
         <v>Yes</v>
       </c>
       <c r="G4" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H4" t="str">
         <v>Yes</v>
       </c>
       <c r="I4" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J4" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K4" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L4" t="str">
-        <v>Full Stack Developer-PLSQL /Java</v>
+        <v>Skipped</v>
       </c>
       <c r="M4" t="str">
-        <v>Oracle</v>
+        <v>.Net MVC Developer</v>
       </c>
       <c r="N4" t="str">
-        <v>3 - 8 years</v>
+        <v>Leading Client</v>
       </c>
       <c r="O4" t="str">
+        <v>1 - 5 years</v>
+      </c>
+      <c r="P4" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P4" t="str">
-        <v>Mumbai</v>
-      </c>
       <c r="Q4" t="str">
+        <v>Udaipur</v>
+      </c>
+      <c r="R4" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R4" t="str">
-        <v>1</v>
-      </c>
       <c r="S4" t="str">
-        <v>18</v>
-      </c>
-      <c r="T4" t="str">
-        <v>PLSQL, prototyping, full stack developer, react, jmeter, ui ux, sql, microservices, java, git, ui, jboss, waterfall, shell scripting, jira, rest, ux, oracle, maven, ai, weblogic, gradle, angular, nlp, full stack, agile, sdlc, soap</v>
+        <v>21</v>
       </c>
       <c r="U4" t="str">
+        <v>mvc, c, web services, sql, software architecture, design, scrum, agile, angularjs, technical documentation, architecture, azure, communication skills</v>
+      </c>
+      <c r="V4" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V4" t="str">
-        <v>IT Services &amp; Consulting</v>
-      </c>
       <c r="W4" t="str">
+        <v>Recruitment / Staffing</v>
+      </c>
+      <c r="X4" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X4" t="str">
+      <c r="Y4" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y4" t="str">
-        <v>3.5</v>
-      </c>
-      <c r="Z4" t="str">
-        <v>Recent graduate or postgraduate with 3-9 years of experience; strong Oracle tech skills including PL/SQL, SQL, and Java; exposure to BFSI domain | Develop and customize Oracle applications; assist in testing and deployment; prepare technical documentation</v>
+      <c r="AA4" t="str">
+        <v>B.Tech/BCA/MCA with strong experience in .Net MVC, C#, and Azure | Design, develop, and maintain ASP.NET MVC applications and SQL databases; create technical documentation; work in a team environment</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-12-26T20:47:56.092Z</v>
+        <v>2025-12-29T20:39:07.254Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -733,7 +733,7 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-senior-developer-infosys-limited-coimbatore-3-to-5-years-220925928001</v>
+        <v>https://www.naukri.com/job-listings-mvc-net-developer-probus-smart-things-pune-0-to-4-years-291225505911</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
@@ -742,69 +742,72 @@
         <v>Yes</v>
       </c>
       <c r="G5" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H5" t="str">
         <v>Yes</v>
       </c>
       <c r="I5" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J5" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K5" t="str">
         <v>External Apply</v>
       </c>
       <c r="L5" t="str">
-        <v>Java Full Stack Senior Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M5" t="str">
-        <v>Infosys</v>
+        <v>MVC .NET Developer</v>
       </c>
       <c r="N5" t="str">
-        <v>3 - 5 years</v>
+        <v>Probus Smart Things</v>
       </c>
       <c r="O5" t="str">
+        <v>0 - 4 years</v>
+      </c>
+      <c r="P5" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P5" t="str">
-        <v>Coimbatore</v>
-      </c>
       <c r="Q5" t="str">
+        <v>Pune</v>
+      </c>
+      <c r="R5" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R5" t="str">
-        <v>1</v>
-      </c>
       <c r="S5" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
       </c>
       <c r="T5" t="str">
-        <v>java development, microservices, spring, apache camel, spring boot, activemq, project management, messaging framework, api integration, rabbitmq, jquery, react.js, java, apache, design patterns, kafka, full stack, api, web application development, project estimation</v>
+        <v>23</v>
       </c>
       <c r="U5" t="str">
+        <v>MVC</v>
+      </c>
+      <c r="V5" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V5" t="str">
+      <c r="W5" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W5" t="str">
+      <c r="X5" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X5" t="str">
+      <c r="Y5" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y5" t="str">
-        <v>3.5</v>
-      </c>
       <c r="Z5" t="str">
-        <v>Bachelor of Engineering with high proficiency in Java Development and experience in Spring Boot, Microservices, and e-commerce web application development | Design, develop, validate, and support technology solutions; gather client requirements and translate them into system specifications; contribute to project estimations and coding across the technical stack</v>
+        <v>2.6</v>
+      </c>
+      <c r="AA5" t="str">
+        <v>Type : . Full time | Experience : . 0 - 4 years</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-12-26T20:48:02.202Z</v>
+        <v>2025-12-29T20:39:11.952Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -813,7 +816,7 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-java-developer-virtusa-consulting-services-pvt-ltd-hyderabad-2-to-7-years-261225920890</v>
+        <v>https://www.naukri.com/job-listings-senior-c-net-angular-full-stack-developer-kolkata-onsite-easy-clinic-kolkata-3-to-7-years-291225015569</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
@@ -822,66 +825,69 @@
         <v>Yes</v>
       </c>
       <c r="G6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H6" t="str">
         <v>Yes</v>
       </c>
       <c r="I6" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K6" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L6" t="str">
-        <v>Java Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Virtusa</v>
+        <v>Senior C# .NET, Angular Full Stack Developer - Kolkata Onsite</v>
       </c>
       <c r="N6" t="str">
-        <v>2 - 7 years</v>
+        <v>Easy Clinic</v>
       </c>
       <c r="O6" t="str">
-        <v>Not Disclosed</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P6" t="str">
-        <v>Hyderabad</v>
+        <v>8-12 Lacs P.A.</v>
       </c>
       <c r="Q6" t="str">
+        <v>Kolkata</v>
+      </c>
+      <c r="R6" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R6" t="str">
-        <v>50+</v>
+      <c r="S6" t="str">
+        <v>4</v>
       </c>
       <c r="T6" t="str">
-        <v>java developer, css, nginx, maven, build tools, weblogic, caching, javascript, redis, sql server, sql, gradle, qa, spring boot, database management, java, jboss, mission critical systems, application security, full stack, software solutions, mvc</v>
+        <v>39</v>
       </c>
       <c r="U6" t="str">
+        <v>C#, Angular, Typescript, .net core, .NET, mvc, Angular Cli, Angular Framework</v>
+      </c>
+      <c r="V6" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V6" t="str">
-        <v>Banking</v>
-      </c>
       <c r="W6" t="str">
+        <v>Software Product</v>
+      </c>
+      <c r="X6" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X6" t="str">
+      <c r="Y6" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y6" t="str">
-        <v>3.7</v>
-      </c>
-      <c r="Z6" t="str">
-        <v>4-6 years of experience in .NET Core development, strong skills in MS SQL Server and ASP.NET Core MVC | Design, develop, and maintain high-performance applications; manage databases and ensure code quality</v>
+      <c r="AA6" t="str">
+        <v>Bachelor's degree in Computer Science or related field; 3+ years of experience as a Full Stack Developer; strong expertise in .NET MVC, C#, and Angular | Design, develop, and maintain scalable web applications; integrate front-end and back-end systems; ensure seamless user experiences | Competitive salary and benefits package</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-12-26T20:48:16.349Z</v>
+        <v>2025-12-29T20:39:16.901Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -890,16 +896,16 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-infosys-limited-hubli-3-to-5-years-290925926272</v>
+        <v>https://www.naukri.com/job-listings-net-aws-developer-virtusa-consulting-services-pvt-ltd-bengaluru-2-to-5-years-291225910208</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
       </c>
       <c r="F7" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G7" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H7" t="str">
         <v>Yes</v>
@@ -911,57 +917,57 @@
         <v>Poor Match</v>
       </c>
       <c r="K7" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L7" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M7" t="str">
-        <v>Infosys</v>
+        <v>.NET AWS Developer</v>
       </c>
       <c r="N7" t="str">
-        <v>3 - 5 years</v>
+        <v>Virtusa</v>
       </c>
       <c r="O7" t="str">
+        <v>2 - 5 years</v>
+      </c>
+      <c r="P7" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P7" t="str">
-        <v>Hubli</v>
-      </c>
       <c r="Q7" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R7" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R7" t="str">
-        <v>1</v>
-      </c>
       <c r="S7" t="str">
-        <v>Less than 10</v>
-      </c>
-      <c r="T7" t="str">
-        <v>spring boot, angular, react.js, java, reactive programming, schema, rest, junit, software testing, maven, manual testing, hibernate, javascript, application development, spring, ui, java code, full stack, architectural patterns, servlets, troubleshooting, aws</v>
+        <v>44</v>
       </c>
       <c r="U7" t="str">
-        <v>Full Stack Developer</v>
+        <v>aws, qa, cloud, rest, apis, devops, distributed systems, terraform, cloud native, code quality</v>
       </c>
       <c r="V7" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Search Engineer</v>
       </c>
       <c r="W7" t="str">
+        <v>Banking</v>
+      </c>
+      <c r="X7" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X7" t="str">
+      <c r="Y7" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y7" t="str">
-        <v>3.5</v>
-      </c>
       <c r="Z7" t="str">
-        <v>MCA, MTech, or Bachelor of Engineering with 3+ years of experience in Java and Angular or React or AWS | Analyze user requirements, design and maintain Java codes, troubleshoot development issues, and implement automated testing</v>
+        <v>3.7</v>
+      </c>
+      <c r="AA7" t="str">
+        <v>4-5 years of experience with AWS, Terraform, C#, and .NET; strong problem-solving skills | Develop and enhance cloud-native services, implement infrastructure-as-code, and collaborate with teams to deliver solutions</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-12-26T20:48:21.450Z</v>
+        <v>2025-12-29T20:39:21.785Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -970,7 +976,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-cgi-information-systems-and-management-consultants-private-limited-bengaluru-3-to-6-years-261225920170</v>
+        <v>https://www.naukri.com/job-listings-senior-net-developer-rudr-consultancy-services-udaipur-3-to-8-years-291225907827</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -979,66 +985,69 @@
         <v>Yes</v>
       </c>
       <c r="G8" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H8" t="str">
         <v>Yes</v>
       </c>
       <c r="I8" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J8" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K8" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L8" t="str">
-        <v>Java full stack Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M8" t="str">
-        <v>CGI</v>
+        <v>Senior .Net Developer</v>
       </c>
       <c r="N8" t="str">
-        <v>3 - 6 years</v>
+        <v>Leading Client</v>
       </c>
       <c r="O8" t="str">
+        <v>3 - 8 years</v>
+      </c>
+      <c r="P8" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P8" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q8" t="str">
+        <v>Udaipur</v>
+      </c>
+      <c r="R8" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R8" t="str">
-        <v>50+</v>
+      <c r="S8" t="str">
+        <v>1</v>
       </c>
       <c r="T8" t="str">
-        <v>Java, rest, restful, streaming data, system programming, full stack developer, microservices, angular, automation, product development, full stack, agile methodologies, scrum, software engineering, agile, aws, programming, financial markets</v>
+        <v>15</v>
       </c>
       <c r="U8" t="str">
+        <v>css, sql, wcf, web programming, linq, c++, web services, ado.net, dbms, bootstrap, t-sql, ajax, jquery, java, asp.net, ssrs, json, html, mysql, phonegap, mvc, c#, python, c, oracle, vb, relational databases, javascript, sql server, angular, web technologies, .net, angularjs</v>
+      </c>
+      <c r="V8" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V8" t="str">
+      <c r="W8" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W8" t="str">
+      <c r="X8" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X8" t="str">
+      <c r="Y8" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y8" t="str">
-        <v>4.0</v>
-      </c>
-      <c r="Z8" t="str">
-        <v>Proficiency in Java, Angular, Microservices, and AWS; experience in financial markets and system programming | Drive technical discussions, maintain CI/CD pipelines, and contribute to software design and development</v>
+      <c r="AA8" t="str">
+        <v>B.Tech/BCA/MCA with 3-10 years experience in .NET technologies and strong SQL knowledge | Deliver solutions for large-scale enterprises using VB.NET/C#, manage tasks, and communicate effectively | Salary is best in the industry</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-12-26T20:48:35.190Z</v>
+        <v>2025-12-29T20:39:26.441Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1047,7 +1056,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-software-engineer-ge-renewable-energy-technologies-private-limited-bengaluru-2-to-5-years-261225926791</v>
+        <v>https://www.naukri.com/job-listings-senior-net-developer-rudr-consultancy-services-udaipur-3-to-8-years-291225908518</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1056,66 +1065,69 @@
         <v>Yes</v>
       </c>
       <c r="G9" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H9" t="str">
         <v>Yes</v>
       </c>
       <c r="I9" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J9" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K9" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L9" t="str">
-        <v>Software Engineer</v>
+        <v>Skipped</v>
       </c>
       <c r="M9" t="str">
-        <v>GE VERNOVA</v>
+        <v>Senior .Net Developer</v>
       </c>
       <c r="N9" t="str">
-        <v>2 - 5 years</v>
+        <v>Leading Client</v>
       </c>
       <c r="O9" t="str">
+        <v>3 - 8 years</v>
+      </c>
+      <c r="P9" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P9" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q9" t="str">
+        <v>Udaipur</v>
+      </c>
+      <c r="R9" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R9" t="str">
-        <v>100+</v>
+      <c r="S9" t="str">
+        <v>1</v>
       </c>
       <c r="T9" t="str">
-        <v>Software Engineer, Java, Postgresql, Ai, User Experience, Full Stack, Restful, React, Machine Learning, Angular, Sql, Restful Apis, Jenkins, Software Development, Front End, Git, Docker, Mysql, Agile, Postgres, Aws, Oracle, Due Diligence, Kubernetes</v>
+        <v>Less than 10</v>
       </c>
       <c r="U9" t="str">
+        <v>jquery, asp.net, phonegap, javascript, web programming, css, c++, web services, ado.net, dbms, t-sql, ajax, sql, java, linux, json, html, mysql, data structures, mvc, wcf, c#, rest, python, c, vb, relational databases, sql server, angular, linq, web technologies, .net, angularjs</v>
+      </c>
+      <c r="V9" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V9" t="str">
-        <v>Power</v>
-      </c>
       <c r="W9" t="str">
+        <v>IT Services &amp; Consulting</v>
+      </c>
+      <c r="X9" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X9" t="str">
+      <c r="Y9" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y9" t="str">
-        <v>4.1</v>
-      </c>
-      <c r="Z9" t="str">
-        <v>Bachelor's degree in Computer Science or STEM with 2-5 years of experience; proficiency in Full Stack .NET (C#) or Java, and modern front-end frameworks like Angular or React | Program and develop software components, maintain code quality, engage in technical discussions, and optimize application performance | Relocation assistance provided</v>
+      <c r="AA9" t="str">
+        <v>B.Tech/BCA/MCA with 3-10 years experience in .NET technologies | Deliver solutions for large-scale enterprises using VB.NET/C#, SQL, and related web technologies | Salary is best in the industry</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-12-26T20:48:49.264Z</v>
+        <v>2025-12-29T20:39:31.540Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1124,7 +1136,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-software-developer-java-web-technologies-oracle-india-pvt-ltd-bengaluru-3-to-6-years-261225908763</v>
+        <v>https://www.naukri.com/job-listings-net-mvc-developer-cjk-knowledgeworks-work-from-office-kilpauk-knowledgeworks-global-kgl-chennai-3-to-7-years-240125009569</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1145,57 +1157,60 @@
         <v>Good Match</v>
       </c>
       <c r="K10" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L10" t="str">
-        <v>Full Stack Software Developer Java/Web Technologies</v>
+        <v>Skipped</v>
       </c>
       <c r="M10" t="str">
-        <v>Oracle</v>
+        <v>.NET &amp; MVC Developer - CJK KnowledgeWorks(Work from Office- Kilpauk)</v>
       </c>
       <c r="N10" t="str">
-        <v>3 - 6 years</v>
+        <v>KnowledgeWorks Global (KGL)</v>
       </c>
       <c r="O10" t="str">
+        <v>3 - 7 years</v>
+      </c>
+      <c r="P10" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P10" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q10" t="str">
+        <v>Chennai( Kilpauk )</v>
+      </c>
+      <c r="R10" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R10" t="str">
-        <v>1</v>
-      </c>
       <c r="S10" t="str">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="T10" t="str">
-        <v>JavaScript, restful, software development, business intelligence, microservices, docker, configuration management, java, git, automation, devops, web technologies, full stack, debugging, software developer</v>
+        <v>50+</v>
       </c>
       <c r="U10" t="str">
+        <v>Net Mvc, asp.net, Asp.Net Core, MVC, MVC Architecture, .Net Core, SQL Server Development, .NET Compact Framework, MVC Framework, Asp.Net Web Api, Asp.Net Core Mvc, ASP.Net MVC, Angular, Fullstack Development, ASP.Net Ajax, .Net, Entity Framework</v>
+      </c>
+      <c r="V10" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V10" t="str">
+      <c r="W10" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W10" t="str">
+      <c r="X10" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X10" t="str">
+      <c r="Y10" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y10" t="str">
-        <v>3.5</v>
-      </c>
       <c r="Z10" t="str">
-        <v>Bachelor's or Master's degree in Computer Science; 4+ years of experience in Java, J2EE, and modern web frameworks; strong knowledge of data structures and algorithms | Develop and debug software applications; perform technical design and code development; contribute to DevOps initiatives</v>
+        <v>2.9</v>
+      </c>
+      <c r="AA10" t="str">
+        <v>Minimum 3 years experience in .Net with MVC framework, proficient in ASP.NET, C#, SQL Server, and Angular JS | Build and maintain .NET applications, ensure code quality, and provide technical support</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-12-26T20:48:53.952Z</v>
+        <v>2025-12-29T20:40:02.479Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1204,7 +1219,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-sarvaha-pune-3-to-8-years-261225917323</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-291225921679</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1225,57 +1240,57 @@
         <v>Good Match</v>
       </c>
       <c r="K11" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L11" t="str">
-        <v>Java Full stack Developer</v>
+        <v>Skipped</v>
       </c>
       <c r="M11" t="str">
-        <v>Sarvaha Systems</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="N11" t="str">
-        <v>3 - 8 years</v>
+        <v>Accenture</v>
       </c>
       <c r="O11" t="str">
+        <v>2 - 5 years</v>
+      </c>
+      <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P11" t="str">
-        <v>Pune</v>
-      </c>
       <c r="Q11" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R11" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R11" t="str">
-        <v>1</v>
-      </c>
       <c r="S11" t="str">
-        <v>100+</v>
-      </c>
-      <c r="T11" t="str">
-        <v>Java, React, Angular, Hibernate, PostgreSQL, Java Full stack Developer, Microservices, Jenkins, Git, Docker, MySQL, MongoDB, Spring boot, Kubernetes</v>
+        <v>Less than 10</v>
       </c>
       <c r="U11" t="str">
+        <v>software engineer, front end, kubernetes, api development, cloud services, restful, software development, version control, javascript, jquery, sql server, sql, docker, restful apis, git, devops, software solutions, mvc, agile, postgres</v>
+      </c>
+      <c r="V11" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V11" t="str">
+      <c r="W11" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W11" t="str">
+      <c r="X11" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X11" t="str">
+      <c r="Y11" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y11" t="str">
-        <v>4.5</v>
-      </c>
       <c r="Z11" t="str">
-        <v>BE/BTech/MTech in CS/IT or MCA with 3+ years of experience in Java and backend services | Design, develop, and maintain scalable applications; collaborate with teams to deliver high-quality solutions | Top-notch remuneration and excellent growth opportunities</v>
+        <v>3.7</v>
+      </c>
+      <c r="AA11" t="str">
+        <v>Minimum 5 years of experience in DevOps with proficiency in cloud services and containerization technologies | Develop and maintain software solutions using C# and .NET Core, design RESTful APIs, and mentor junior team members</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-12-26T20:49:07.607Z</v>
+        <v>2025-12-29T20:40:07.217Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1284,7 +1299,7 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-261225918782</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-291225919029</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
@@ -1308,51 +1323,54 @@
         <v>External Apply</v>
       </c>
       <c r="L12" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M12" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N12" t="str">
-        <v>2 - 5 years</v>
-      </c>
       <c r="O12" t="str">
+        <v>3 - 8 years</v>
+      </c>
+      <c r="P12" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P12" t="str">
-        <v>Chennai</v>
-      </c>
       <c r="Q12" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R12" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R12" t="str">
+      <c r="S12" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T12" t="str">
-        <v>software engineer, application developer, css, version control, business processes, hibernate, javascript, nosql, sql, database management, java, git, web technologies, full stack, software solutions, construction, html, agile, nosql databases</v>
-      </c>
       <c r="U12" t="str">
-        <v>Full Stack Developer</v>
+        <v>software engineer, front end, kubernetes, application developer, restful, react, sql server, sql, microservices, docker, angular, restful apis, git, devops, oops, kafka, jenkins, scrum, mvc, agile, aws, mongodb, architecture, azure</v>
       </c>
       <c r="V12" t="str">
+        <v>Search Engineer</v>
+      </c>
+      <c r="W12" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W12" t="str">
+      <c r="X12" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X12" t="str">
+      <c r="Y12" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y12" t="str">
+      <c r="Z12" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z12" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in web technologies and frameworks | Develop custom software solutions, collaborate with stakeholders, and mentor junior team members</v>
+      <c r="AA12" t="str">
+        <v>Minimum 3 years experience in ASP.NET MVC and strong understanding of .NET Core, Microservices, and RESTful APIs | Develop custom software solutions, engage in design and coding, participate in team discussions, and conduct code reviews</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-12-26T20:49:12.849Z</v>
+        <v>2025-12-29T20:40:12.565Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1361,13 +1379,13 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-261225917853</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-291225921439</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
       </c>
       <c r="F13" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G13" t="str">
         <v>Yes</v>
@@ -1376,60 +1394,63 @@
         <v>Yes</v>
       </c>
       <c r="I13" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J13" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K13" t="str">
         <v>External Apply</v>
       </c>
       <c r="L13" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M13" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N13" t="str">
+      <c r="O13" t="str">
         <v>2 - 5 years</v>
       </c>
-      <c r="O13" t="str">
+      <c r="P13" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P13" t="str">
-        <v>Chennai</v>
-      </c>
       <c r="Q13" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R13" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R13" t="str">
+      <c r="S13" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T13" t="str">
-        <v>software engineer, software development, full stack development, version control, programming principles, sql, spring boot, database management, java, git, design, full stack, software solutions, debugging, agile, programming</v>
-      </c>
       <c r="U13" t="str">
-        <v>Full Stack Developer</v>
+        <v>software engineer, kubernetes, react, iac, microservices, docker, tensorflow, iam, devops, pytorch, debugging, mvc, graphql, architecture, azure, front end, python, ai, aws sagemaker, angular, kafka, full stack, terraform, agile, aws</v>
       </c>
       <c r="V13" t="str">
+        <v>Blockchain Quality Assurance Engineer</v>
+      </c>
+      <c r="W13" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W13" t="str">
+      <c r="X13" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X13" t="str">
-        <v>Software Development</v>
-      </c>
       <c r="Y13" t="str">
+        <v>Quality Assurance and Testing</v>
+      </c>
+      <c r="Z13" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z13" t="str">
-        <v>Minimum 5 years experience in Java Standard Edition; proficiency in object-oriented programming; familiarity with Agile methodologies | Develop custom software solutions; collaborate with cross-functional teams; mentor junior team members</v>
+      <c r="AA13" t="str">
+        <v>Bachelor's degree in computer science or related field; 5-12 years of full-stack development experience with strong proficiency in .NET and Python; familiarity with AI/ML integration and multi-cloud environments | Develop and deploy custom software solutions; lead AI-driven solution design; collaborate with teams for application development and integration</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-12-26T20:49:17.694Z</v>
+        <v>2025-12-29T20:40:17.268Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1438,13 +1459,13 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225918403</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-291225923684</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
       </c>
       <c r="F14" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G14" t="str">
         <v>Yes</v>
@@ -1453,60 +1474,63 @@
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K14" t="str">
         <v>External Apply</v>
       </c>
       <c r="L14" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M14" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N14" t="str">
+      <c r="O14" t="str">
         <v>2 - 5 years</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P14" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P14" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q14" t="str">
+        <v>Pune</v>
+      </c>
+      <c r="R14" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R14" t="str">
+      <c r="S14" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T14" t="str">
-        <v>software engineer, restful, software development, web services, version control, react, amazon web services, microservices, spring boot, database management, java, git, postgresql, api design, full stack, software solutions, mysql, agile, aws</v>
-      </c>
       <c r="U14" t="str">
-        <v>Full Stack Developer</v>
+        <v>software engineer, kubernetes, react, iac, microservices, docker, tensorflow, iam, devops, pytorch, debugging, mvc, graphql, architecture, azure, front end, python, ai, aws sagemaker, angular, kafka, full stack, terraform, agile, aws</v>
       </c>
       <c r="V14" t="str">
+        <v>Blockchain Quality Assurance Engineer</v>
+      </c>
+      <c r="W14" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W14" t="str">
+      <c r="X14" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X14" t="str">
-        <v>Software Development</v>
-      </c>
       <c r="Y14" t="str">
+        <v>Quality Assurance and Testing</v>
+      </c>
+      <c r="Z14" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z14" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with skills in AWS, Spring Boot, and React.js | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+      <c r="AA14" t="str">
+        <v>5+ years of experience in .NET Full Stack Development with strong skills in Python and front-end frameworks like React or Angular | Develop and enhance custom software solutions, lead AI-driven design, and implement multi-cloud applications</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-12-26T20:49:22.390Z</v>
+        <v>2025-12-29T20:40:21.946Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1515,7 +1539,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225917923</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-2-to-5-years-291225925315</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1524,66 +1548,69 @@
         <v>Yes</v>
       </c>
       <c r="G15" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H15" t="str">
         <v>Yes</v>
       </c>
       <c r="I15" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K15" t="str">
         <v>External Apply</v>
       </c>
       <c r="L15" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M15" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N15" t="str">
+      <c r="O15" t="str">
         <v>2 - 5 years</v>
       </c>
-      <c r="O15" t="str">
+      <c r="P15" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P15" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q15" t="str">
+        <v>Navi Mumbai</v>
+      </c>
+      <c r="R15" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R15" t="str">
+      <c r="S15" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T15" t="str">
-        <v>software engineer, restful, software development, web services, version control, react, amazon web services, microservices, spring boot, database management, java, git, postgresql, api design, full stack, software solutions, mysql, agile, aws</v>
-      </c>
       <c r="U15" t="str">
+        <v>software engineer, front end, application developer, css, full stack development, version control, business processes, user experience, javascript, sql server, sql, back end, git, full stack, software solutions, debugging, construction, html, agile</v>
+      </c>
+      <c r="V15" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V15" t="str">
+      <c r="W15" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W15" t="str">
+      <c r="X15" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X15" t="str">
+      <c r="Y15" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y15" t="str">
+      <c r="Z15" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z15" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development; proficiency in Java, React.js, Spring Boot, and AWS | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+      <c r="AA15" t="str">
+        <v>Minimum . 2 year(s) of experience is required. Educational Qualification : 15 years full time education. Summary :As an Application Developer,you will engage in the design,construction,and configuration of applications tailored to fulfill specific business processes and application requirements | Required active participation / contribution in team discussions</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-12-26T20:49:27.122Z</v>
+        <v>2025-12-29T20:40:26.683Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1592,7 +1619,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-261225918695</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-3-to-8-years-291225923728</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1616,51 +1643,54 @@
         <v>External Apply</v>
       </c>
       <c r="L16" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M16" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M16" t="str">
+      <c r="N16" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N16" t="str">
-        <v>2 - 5 years</v>
-      </c>
       <c r="O16" t="str">
+        <v>3 - 8 years</v>
+      </c>
+      <c r="P16" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P16" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q16" t="str">
+        <v>Pune</v>
+      </c>
+      <c r="R16" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R16" t="str">
+      <c r="S16" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T16" t="str">
-        <v>software engineer, api development, restful, web services, full stack development, version control, react, amazon web services, sql, microservices, spring boot, database management, java, git, full stack, software solutions, agile, aws, architecture</v>
-      </c>
       <c r="U16" t="str">
+        <v>software engineer, restful, full stack development, version control, sql server, sql, web development frameworks, angular, database management, git, api design, full stack, agile methodologies, software solutions, debugging, web development, agile</v>
+      </c>
+      <c r="V16" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V16" t="str">
+      <c r="W16" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W16" t="str">
+      <c r="X16" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X16" t="str">
+      <c r="Y16" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y16" t="str">
+      <c r="Z16" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z16" t="str">
-        <v>Minimum 5 years experience in Java Full Stack Development, proficiency in AWS, Spring Boot, and React.js | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+      <c r="AA16" t="str">
+        <v>Minimum 3 years experience in .Net Full Stack Development with proficiency in ASP.NET and Angular | Develop custom software solutions, collaborate with teams, and troubleshoot software issues</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-12-26T20:49:31.843Z</v>
+        <v>2025-12-29T20:40:31.275Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1669,7 +1699,7 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-261225918663</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-2-to-5-years-291225924738</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
@@ -1678,66 +1708,69 @@
         <v>Yes</v>
       </c>
       <c r="G17" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H17" t="str">
         <v>Yes</v>
       </c>
       <c r="I17" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J17" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K17" t="str">
         <v>External Apply</v>
       </c>
       <c r="L17" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M17" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M17" t="str">
+      <c r="N17" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N17" t="str">
-        <v>3 - 8 years</v>
-      </c>
       <c r="O17" t="str">
+        <v>2 - 5 years</v>
+      </c>
+      <c r="P17" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P17" t="str">
-        <v>Chennai</v>
-      </c>
       <c r="Q17" t="str">
+        <v>Navi Mumbai</v>
+      </c>
+      <c r="R17" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R17" t="str">
+      <c r="S17" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T17" t="str">
-        <v>software engineer, application developer, full stack development, version control, business processes, react, sql, spring boot, database management, java, git, design, full stack, software solutions, construction, agile, architecture</v>
-      </c>
       <c r="U17" t="str">
+        <v>software engineer, front end, application developer, restful, web services, version control, react, sql server, sql, angular, database management, restful apis, git, business process, apis, full stack, software solutions, agile</v>
+      </c>
+      <c r="V17" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V17" t="str">
+      <c r="W17" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W17" t="str">
+      <c r="X17" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X17" t="str">
+      <c r="Y17" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y17" t="str">
+      <c r="Z17" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z17" t="str">
-        <v>Minimum 3 years experience in Java Full Stack Development with proficiency in modern frameworks | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
+      <c r="AA17" t="str">
+        <v>Minimum . 2 year(s) of experience is required. Educational Qualification : 15 years full time education. Summary :As an Application Developer,you will design,build,and configure applications to meet business process and application requirements | A 15 years full time education is required. . Qualification 15 years full time education | Good To Have</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-12-26T20:49:36.510Z</v>
+        <v>2025-12-29T20:40:36.010Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1746,13 +1779,13 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bhubaneswar-2-to-5-years-261225918260</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-3-to-8-years-291225924406</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
       </c>
       <c r="F18" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G18" t="str">
         <v>No</v>
@@ -1761,7 +1794,7 @@
         <v>Yes</v>
       </c>
       <c r="I18" t="str">
-        <v>3/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J18" t="str">
         <v>Poor Match</v>
@@ -1770,51 +1803,54 @@
         <v>External Apply</v>
       </c>
       <c r="L18" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M18" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M18" t="str">
+      <c r="N18" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N18" t="str">
-        <v>2 - 5 years</v>
-      </c>
       <c r="O18" t="str">
+        <v>3 - 8 years</v>
+      </c>
+      <c r="P18" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P18" t="str">
-        <v>Bhubaneswar</v>
-      </c>
       <c r="Q18" t="str">
+        <v>Navi Mumbai</v>
+      </c>
+      <c r="R18" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R18" t="str">
+      <c r="S18" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T18" t="str">
-        <v>software engineer, front end, css, restful, software development, javascript, microservices, back end, software development lifecycle, java, restful apis, git, microservices architecture, full stack, construction, agile, architecture</v>
-      </c>
       <c r="U18" t="str">
+        <v>software engineer, front end, application developer, cloud services, restful, web services, business processes, react, sql server, sql, cloud, angular, database management, restful apis, business process, apis, full stack, construction</v>
+      </c>
+      <c r="V18" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V18" t="str">
+      <c r="W18" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W18" t="str">
+      <c r="X18" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X18" t="str">
+      <c r="Y18" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y18" t="str">
+      <c r="Z18" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z18" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end and back-end technologies | Develop custom software solutions, collaborate with teams, and mentor junior members</v>
+      <c r="AA18" t="str">
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-12-26T20:49:41.268Z</v>
+        <v>2025-12-29T20:40:40.696Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1823,13 +1859,13 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-261225918784</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-3-to-5-years-291225923238</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
       </c>
       <c r="F19" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G19" t="str">
         <v>Yes</v>
@@ -1838,60 +1874,63 @@
         <v>Yes</v>
       </c>
       <c r="I19" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J19" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K19" t="str">
         <v>External Apply</v>
       </c>
       <c r="L19" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M19" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M19" t="str">
+      <c r="N19" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N19" t="str">
-        <v>3 - 8 years</v>
-      </c>
       <c r="O19" t="str">
+        <v>3 - 5 years</v>
+      </c>
+      <c r="P19" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P19" t="str">
-        <v>Bengaluru</v>
-      </c>
       <c r="Q19" t="str">
+        <v>Pune</v>
+      </c>
+      <c r="R19" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R19" t="str">
+      <c r="S19" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T19" t="str">
-        <v>software engineer, version control, react, amazon web services, user experience, microservices, web development frameworks, spring boot, database management, java, git, data modeling, full stack, software solutions, web development, agile, aws</v>
-      </c>
       <c r="U19" t="str">
-        <v>Full Stack Developer</v>
+        <v>software engineer, front end, kubernetes, python, predictive analytics, ai, react, devops engineer, microservices, docker, angular, iam, spark, compliance, kafka, full stack, mvc, hadoop, graphql, big data, aws, architecture, azure</v>
       </c>
       <c r="V19" t="str">
+        <v>Blockchain Quality Assurance Engineer</v>
+      </c>
+      <c r="W19" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W19" t="str">
+      <c r="X19" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X19" t="str">
-        <v>Software Development</v>
-      </c>
       <c r="Y19" t="str">
+        <v>Quality Assurance and Testing</v>
+      </c>
+      <c r="Z19" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z19" t="str">
-        <v>Minimum 3 years experience in Java Full Stack Development, proficiency in React.js, Spring Boot, and AWS | Develop custom software solutions, collaborate with teams to gather requirements, and mentor junior members</v>
+      <c r="AA19" t="str">
+        <v>12 to 20+ years in enterprise architecture with strong .NET Core, Python, and AI integration skills | Design and implement application-heavy enterprise architectures across multi-cloud environments</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-12-26T20:49:46.013Z</v>
+        <v>2025-12-29T20:40:45.777Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1900,13 +1939,13 @@
         <v>19/20</v>
       </c>
       <c r="D20" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-261225917858</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-5-years-291225921956</v>
       </c>
       <c r="E20" t="str">
         <v>Yes</v>
       </c>
       <c r="F20" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G20" t="str">
         <v>Yes</v>
@@ -1915,60 +1954,63 @@
         <v>Yes</v>
       </c>
       <c r="I20" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J20" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K20" t="str">
         <v>External Apply</v>
       </c>
       <c r="L20" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M20" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M20" t="str">
+      <c r="N20" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N20" t="str">
-        <v>3 - 8 years</v>
-      </c>
       <c r="O20" t="str">
+        <v>3 - 5 years</v>
+      </c>
+      <c r="P20" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P20" t="str">
-        <v>Gurugram</v>
-      </c>
       <c r="Q20" t="str">
+        <v>Bengaluru</v>
+      </c>
+      <c r="R20" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R20" t="str">
+      <c r="S20" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T20" t="str">
-        <v>software engineer, application developer, restful, ux, version control, business processes, react, sql, web development frameworks, back end, database management, java, git, ui, full stack, debugging, construction, web development, ux design</v>
-      </c>
       <c r="U20" t="str">
-        <v>Full Stack Developer</v>
+        <v>software engineer, front end, kubernetes, python, predictive analytics, ai, react, devops engineer, microservices, docker, angular, iam, spark, compliance, kafka, full stack, mvc, hadoop, graphql, big data, aws, architecture, azure</v>
       </c>
       <c r="V20" t="str">
+        <v>Blockchain Quality Assurance Engineer</v>
+      </c>
+      <c r="W20" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W20" t="str">
+      <c r="X20" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X20" t="str">
-        <v>Software Development</v>
-      </c>
       <c r="Y20" t="str">
+        <v>Quality Assurance and Testing</v>
+      </c>
+      <c r="Z20" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z20" t="str">
-        <v>Minimum 3 years experience in Java Full Stack Development; proficiency in React.js; 15 years full-time education | Design, build, and configure applications; participate in testing and debugging; assist in documentation</v>
+      <c r="AA20" t="str">
+        <v>12 to 20+ years in enterprise architecture with strong .NET Core, Python, and AI integration skills | Design and implement application-heavy enterprise architectures across multi-cloud environments, lead full-stack development, and ensure seamless system integrations</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-12-26T20:49:53.162Z</v>
+        <v>2025-12-29T20:40:50.483Z</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1977,7 +2019,7 @@
         <v>20/20</v>
       </c>
       <c r="D21" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-3-to-8-years-261225917771</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-291225923006</v>
       </c>
       <c r="E21" t="str">
         <v>Yes</v>
@@ -1986,13 +2028,13 @@
         <v>No</v>
       </c>
       <c r="G21" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H21" t="str">
         <v>Yes</v>
       </c>
       <c r="I21" t="str">
-        <v>2/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J21" t="str">
         <v>Poor Match</v>
@@ -2001,51 +2043,54 @@
         <v>External Apply</v>
       </c>
       <c r="L21" t="str">
+        <v>Skipped</v>
+      </c>
+      <c r="M21" t="str">
         <v>Custom Software Engineer</v>
       </c>
-      <c r="M21" t="str">
+      <c r="N21" t="str">
         <v>Accenture</v>
       </c>
-      <c r="N21" t="str">
-        <v>3 - 8 years</v>
-      </c>
       <c r="O21" t="str">
+        <v>2 - 5 years</v>
+      </c>
+      <c r="P21" t="str">
         <v>Not Disclosed</v>
       </c>
-      <c r="P21" t="str">
-        <v>Navi Mumbai</v>
-      </c>
       <c r="Q21" t="str">
+        <v>Pune</v>
+      </c>
+      <c r="R21" t="str">
         <v>1 day ago</v>
       </c>
-      <c r="R21" t="str">
+      <c r="S21" t="str">
         <v>Less than 10</v>
       </c>
-      <c r="T21" t="str">
-        <v>software engineer, application developer, cloud services, version control, business processes, sql, web development frameworks, cloud, database management, java, git, business process, full stack, debugging, construction, web development</v>
-      </c>
       <c r="U21" t="str">
+        <v>software engineer, rest, software development, web services, microsoft dynamics, user experience, javascript, sql server, sales, sql, marketing, active directory, software solutions, http, agile, ssis, dynamics 365, soap, architecture, azure, crm</v>
+      </c>
+      <c r="V21" t="str">
         <v>Full Stack Developer</v>
       </c>
-      <c r="V21" t="str">
+      <c r="W21" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
-      <c r="W21" t="str">
+      <c r="X21" t="str">
         <v>Full Time, Permanent</v>
       </c>
-      <c r="X21" t="str">
+      <c r="Y21" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Y21" t="str">
+      <c r="Z21" t="str">
         <v>3.7</v>
       </c>
-      <c r="Z21" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development and 15 years of full-time education | Design, build, and configure applications to meet business requirements, collaborate with teams, and ensure application performance</v>
+      <c r="AA21" t="str">
+        <v>Minimum 5 years experience in Microsoft Dynamics CRM Technical and 15 years full-time education | Develop and customize Microsoft Dynamics 365 applications, manage timelines, and ensure quality</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added mising changes of Db
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-12-29T20:38:51.669Z</v>
+        <v>2026-01-01T17:43:43.310Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-net-developer-wpf-maui-web-api-iot-gvrai-technologies-bengaluru-0-to-3-years-291225028590</v>
+        <v>https://www.naukri.com/job-listings-junior-java-developer-miko-mumbai-0-to-3-years-311225909298</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -523,19 +523,19 @@
         <v>Skipped</v>
       </c>
       <c r="M2" t="str">
-        <v>.NET Developer (WPF / MAUI / Web API / IoT)</v>
+        <v>Junior Java Developer</v>
       </c>
       <c r="N2" t="str">
-        <v>Gvrai Technologies</v>
+        <v>Miko</v>
       </c>
       <c r="O2" t="str">
         <v>0 - 3 years</v>
       </c>
       <c r="P2" t="str">
-        <v>12-36 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q2" t="str">
-        <v>Bengaluru</v>
+        <v>Mumbai</v>
       </c>
       <c r="R2" t="str">
         <v>1 day ago</v>
@@ -544,16 +544,16 @@
         <v>1</v>
       </c>
       <c r="T2" t="str">
-        <v>50+</v>
+        <v>100+</v>
       </c>
       <c r="U2" t="str">
-        <v>C#, Asp.Net Core, MAUI, WPF, Entity Framework Core, English, .Net Core, C++, Esp32, Sql Server, Microsoft Azure, IoT</v>
+        <v>linux, monolithic, orm, multithread programming, sql database, kubernetes, application development lifecycle, scala, hosting, hibernate, docker, ansible, sql, spring, testing frameworks, java, spark, devops, jpa, mysql, python, rpc, akka, serialization, puppet, servlets</v>
       </c>
       <c r="V2" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W2" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Education / Training</v>
       </c>
       <c r="X2" t="str">
         <v>Full Time, Permanent</v>
@@ -561,13 +561,16 @@
       <c r="Y2" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Z2" t="str">
+        <v>3.4</v>
+      </c>
       <c r="AA2" t="str">
-        <v>Expertise in C# and .NET 6+, with hands-on experience in ASP.NET Core Web API and Entity Framework Core | Develop and maintain applications using .NET technologies, including Azure and SQL Server</v>
+        <v>Proficiency in Java, Linux, and distributed application development lifecycle | Design and develop core system features and collaborate with cross-functional teams</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-12-29T20:38:56.594Z</v>
+        <v>2026-01-01T17:43:48.200Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -576,46 +579,46 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-net-mvc-developer-rudr-consultancy-services-udaipur-1-to-3-years-291225907594</v>
+        <v>https://www.naukri.com/job-listings-java-developer-sutherland-global-services-inc-chennai-1-to-4-years-311225501807</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
       </c>
       <c r="F3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G3" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H3" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I3" t="str">
-        <v>2/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J3" t="str">
         <v>Poor Match</v>
       </c>
       <c r="K3" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L3" t="str">
         <v>Skipped</v>
       </c>
       <c r="M3" t="str">
-        <v>.Net Mvc Developer</v>
+        <v>Java Developer</v>
       </c>
       <c r="N3" t="str">
-        <v>Leading Client</v>
+        <v>Sutherland Global Services Inc</v>
       </c>
       <c r="O3" t="str">
-        <v>1 - 3 years</v>
+        <v>1 - 4 years</v>
       </c>
       <c r="P3" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q3" t="str">
-        <v>Udaipur</v>
+        <v>Chennai</v>
       </c>
       <c r="R3" t="str">
         <v>1 day ago</v>
@@ -624,10 +627,10 @@
         <v>1</v>
       </c>
       <c r="T3" t="str">
-        <v>42</v>
+        <v>100+</v>
       </c>
       <c r="U3" t="str">
-        <v>sql, asp.net, mvc, entity framework, .net core, css, web services, ado.net, bootstrap, ajax, jquery, java, oops, json, html, web api, wcf, c#, mvc framework, asp.net mvc, mvc architecture, mvc implementation, sql server, javascript, angular, linq, .net, angularjs, asp</v>
+        <v>Maven, Hibernate, Web services, jQuery, Version control, GIT, Coding, PLSQL, Regression testing</v>
       </c>
       <c r="V3" t="str">
         <v>Full Stack Developer</v>
@@ -641,13 +644,16 @@
       <c r="Y3" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Z3" t="str">
+        <v>3.4</v>
+      </c>
       <c r="AA3" t="str">
-        <v>1-3 years experience in .NET, MVC, ASP, Entity Frameworks, C#; BTech, BCA, or MCA degree | Develop software solutions using .NET infrastructure, reformulate existing code, and deliver solutions for large-scale enterprises | Salary is best in the industry</v>
+        <v>Graduation / Post Graduation in Computer Science / Related Engineering | Expertise in Spring Batch,PL / SQL,Drools,RabbitMQ,Kafka streaming will be added advantage. | In this role,you should be a team player with a keen eye for detail and problem-solving skills | Knowledge of CI / CD systems,preferably Jenkins.</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-12-29T20:39:02.351Z</v>
+        <v>2026-01-01T17:43:52.960Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -656,7 +662,7 @@
         <v>3/20</v>
       </c>
       <c r="D4" t="str">
-        <v>https://www.naukri.com/job-listings-net-mvc-developer-rudr-consultancy-services-udaipur-jaipur-1-to-5-years-291225916612</v>
+        <v>https://www.naukri.com/job-listings-chief-technology-officer-vice-president-full-stack-development-benovymed-healthcare-private-ltd-hyderabad-2-to-7-years-311225908732</v>
       </c>
       <c r="E4" t="str">
         <v>Yes</v>
@@ -665,16 +671,16 @@
         <v>Yes</v>
       </c>
       <c r="G4" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H4" t="str">
         <v>Yes</v>
       </c>
       <c r="I4" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J4" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K4" t="str">
         <v>Direct Apply</v>
@@ -683,34 +689,34 @@
         <v>Skipped</v>
       </c>
       <c r="M4" t="str">
-        <v>.Net MVC Developer</v>
+        <v>Chief Technology Officer/Vice President - Full Stack Development</v>
       </c>
       <c r="N4" t="str">
-        <v>Leading Client</v>
+        <v>Benovymed Healthcare Private Ltd</v>
       </c>
       <c r="O4" t="str">
-        <v>1 - 5 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P4" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q4" t="str">
-        <v>Udaipur</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R4" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S4" t="str">
-        <v>21</v>
+        <v>50+</v>
       </c>
       <c r="U4" t="str">
-        <v>mvc, c, web services, sql, software architecture, design, scrum, agile, angularjs, technical documentation, architecture, azure, communication skills</v>
+        <v>Full Stack Development, AngularJS, MEAN, Java, NoSQL, Django, Full Stack, LAMP, React.js, AWS, CTO, Python</v>
       </c>
       <c r="V4" t="str">
-        <v>Full Stack Developer</v>
+        <v>Head - Engineering</v>
       </c>
       <c r="W4" t="str">
-        <v>Recruitment / Staffing</v>
+        <v>Medical Services / Hospital</v>
       </c>
       <c r="X4" t="str">
         <v>Full Time, Permanent</v>
@@ -719,12 +725,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA4" t="str">
-        <v>B.Tech/BCA/MCA with strong experience in .Net MVC, C#, and Azure | Design, develop, and maintain ASP.NET MVC applications and SQL databases; create technical documentation; work in a team environment</v>
+        <v>B.Tech in CSE/IT/ECE with 2-10 years of experience in full-stack development and startup environments | Develop and architect a scalable SaaS Cloud Platform, manage end-to-end product development, and ensure cross-platform optimization</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-12-29T20:39:07.254Z</v>
+        <v>2026-01-01T17:44:06.697Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -733,7 +739,7 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-mvc-net-developer-probus-smart-things-pune-0-to-4-years-291225505911</v>
+        <v>https://www.naukri.com/job-listings-python-django-developer-starclinch-new-delhi-1-to-3-years-311225909133</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
@@ -745,34 +751,34 @@
         <v>Yes</v>
       </c>
       <c r="H5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I5" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J5" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K5" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L5" t="str">
         <v>Skipped</v>
       </c>
       <c r="M5" t="str">
-        <v>MVC .NET Developer</v>
+        <v>Python/ Django Developer</v>
       </c>
       <c r="N5" t="str">
-        <v>Probus Smart Things</v>
+        <v>Starclinch</v>
       </c>
       <c r="O5" t="str">
-        <v>0 - 4 years</v>
+        <v>1 - 3 years</v>
       </c>
       <c r="P5" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q5" t="str">
-        <v>Pune</v>
+        <v>New Delhi</v>
       </c>
       <c r="R5" t="str">
         <v>1 day ago</v>
@@ -781,16 +787,16 @@
         <v>1</v>
       </c>
       <c r="T5" t="str">
-        <v>23</v>
+        <v>100+</v>
       </c>
       <c r="U5" t="str">
-        <v>MVC</v>
+        <v>Python, css, confluence, web application, dbms, bitbucket, ajax, jquery, sql, docker, java, git, computer science, gcp, asp.net, jenkins, json, html, mysql, jira, c#, rest, ms azure, github, software testing, javascript, sql server, redmine, django, web technologies, gitlab, aws</v>
       </c>
       <c r="V5" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W5" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Industrial Equipment / Machinery</v>
       </c>
       <c r="X5" t="str">
         <v>Full Time, Permanent</v>
@@ -799,15 +805,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z5" t="str">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="AA5" t="str">
-        <v>Type : . Full time | Experience : . 0 - 4 years</v>
+        <v>1-3 years of experience in software development with strong skills in Python and Django | Develop and maintain complex software, write clean and testable code, and manage end-to-end project responsibilities</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-12-29T20:39:11.952Z</v>
+        <v>2026-01-01T17:44:12.380Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -816,7 +822,7 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-senior-c-net-angular-full-stack-developer-kolkata-onsite-easy-clinic-kolkata-3-to-7-years-291225015569</v>
+        <v>https://www.naukri.com/job-listings-full-stack-developer-3-yrs-navsan-hyderabad-3-to-6-years-311225026777</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
@@ -825,16 +831,16 @@
         <v>Yes</v>
       </c>
       <c r="G6" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H6" t="str">
         <v>Yes</v>
       </c>
       <c r="I6" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K6" t="str">
         <v>Direct Apply</v>
@@ -843,37 +849,37 @@
         <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Senior C# .NET, Angular Full Stack Developer - Kolkata Onsite</v>
+        <v>Full Stack Developer 3 Yrs+</v>
       </c>
       <c r="N6" t="str">
-        <v>Easy Clinic</v>
+        <v>Navsan</v>
       </c>
       <c r="O6" t="str">
-        <v>3 - 7 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P6" t="str">
-        <v>8-12 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q6" t="str">
-        <v>Kolkata</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R6" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S6" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T6" t="str">
-        <v>39</v>
+        <v>100+</v>
       </c>
       <c r="U6" t="str">
-        <v>C#, Angular, Typescript, .net core, .NET, mvc, Angular Cli, Angular Framework</v>
+        <v>Node.Js, React.Js, Java, Fullstack Development, Full Stack, Angular, Python</v>
       </c>
       <c r="V6" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W6" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="X6" t="str">
         <v>Full Time, Permanent</v>
@@ -882,12 +888,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA6" t="str">
-        <v>Bachelor's degree in Computer Science or related field; 3+ years of experience as a Full Stack Developer; strong expertise in .NET MVC, C#, and Angular | Design, develop, and maintain scalable web applications; integrate front-end and back-end systems; ensure seamless user experiences | Competitive salary and benefits package</v>
+        <v>Strong expertise in React, Angular, Node.js, and Python; Bachelor's degree in Computer Science or related field | Design, develop, and maintain scalable web applications; Build backend services and APIs; Ensure application security and performance optimization</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-12-29T20:39:16.901Z</v>
+        <v>2026-01-01T17:44:43.818Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -896,13 +902,13 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-net-aws-developer-virtusa-consulting-services-pvt-ltd-bengaluru-2-to-5-years-291225910208</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-software-engineer-mco-mycompliance-india-hyderabad-3-to-6-years-301225025997</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
       </c>
       <c r="F7" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G7" t="str">
         <v>Yes</v>
@@ -911,10 +917,10 @@
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K7" t="str">
         <v>Direct Apply</v>
@@ -923,34 +929,37 @@
         <v>Skipped</v>
       </c>
       <c r="M7" t="str">
-        <v>.NET AWS Developer</v>
+        <v>Java Full Stack Developer || Software Engineer</v>
       </c>
       <c r="N7" t="str">
-        <v>Virtusa</v>
+        <v>MCO Mycompliance India</v>
       </c>
       <c r="O7" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P7" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q7" t="str">
-        <v>Bengaluru</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R7" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S7" t="str">
-        <v>44</v>
+        <v>8</v>
+      </c>
+      <c r="T7" t="str">
+        <v>100+</v>
       </c>
       <c r="U7" t="str">
-        <v>aws, qa, cloud, rest, apis, devops, distributed systems, terraform, cloud native, code quality</v>
+        <v>Hibernate, Java Fullstack, Spring, React, Multithreading, Orm Tool, Java, J2Ee, ORM, Angular, SQL, NoSQL, Oracle</v>
       </c>
       <c r="V7" t="str">
-        <v>Search Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W7" t="str">
-        <v>Banking</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="X7" t="str">
         <v>Full Time, Permanent</v>
@@ -958,16 +967,13 @@
       <c r="Y7" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z7" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA7" t="str">
-        <v>4-5 years of experience with AWS, Terraform, C#, and .NET; strong problem-solving skills | Develop and enhance cloud-native services, implement infrastructure-as-code, and collaborate with teams to deliver solutions</v>
+        <v>Degree in Engineering/Computer Science with 8-12 years of experience in Java and J2EE technologies | Design, code, and test software; develop enterprise applications; collaborate on technical specifications</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-12-29T20:39:21.785Z</v>
+        <v>2026-01-01T17:45:19.185Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -976,7 +982,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-senior-net-developer-rudr-consultancy-services-udaipur-3-to-8-years-291225907827</v>
+        <v>https://www.naukri.com/job-listings-senior-full-stack-developer-java-vue-js-transunion-pune-chennai-3-to-9-years-311225502334</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -985,37 +991,37 @@
         <v>Yes</v>
       </c>
       <c r="G8" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H8" t="str">
         <v>Yes</v>
       </c>
       <c r="I8" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J8" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K8" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L8" t="str">
         <v>Skipped</v>
       </c>
       <c r="M8" t="str">
-        <v>Senior .Net Developer</v>
+        <v>Senior Full Stack Developer (Java + Vue.js)</v>
       </c>
       <c r="N8" t="str">
-        <v>Leading Client</v>
+        <v>Transunion</v>
       </c>
       <c r="O8" t="str">
-        <v>3 - 8 years</v>
+        <v>3 - 9 years</v>
       </c>
       <c r="P8" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q8" t="str">
-        <v>Udaipur</v>
+        <v>Pune</v>
       </c>
       <c r="R8" t="str">
         <v>1 day ago</v>
@@ -1024,10 +1030,10 @@
         <v>1</v>
       </c>
       <c r="T8" t="str">
-        <v>15</v>
+        <v>50+</v>
       </c>
       <c r="U8" t="str">
-        <v>css, sql, wcf, web programming, linq, c++, web services, ado.net, dbms, bootstrap, t-sql, ajax, jquery, java, asp.net, ssrs, json, html, mysql, phonegap, mvc, c#, python, c, oracle, vb, relational databases, javascript, sql server, angular, web technologies, .net, angularjs</v>
+        <v>Maven, Hibernate, Automation, Backend, Integration testing, Javascript, JDBC, JPA, SQL, CSS3</v>
       </c>
       <c r="V8" t="str">
         <v>Full Stack Developer</v>
@@ -1041,13 +1047,16 @@
       <c r="Y8" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Z8" t="str">
+        <v>3.7</v>
+      </c>
       <c r="AA8" t="str">
-        <v>B.Tech/BCA/MCA with 3-10 years experience in .NET technologies and strong SQL knowledge | Deliver solutions for large-scale enterprises using VB.NET/C#, manage tasks, and communicate effectively | Salary is best in the industry</v>
+        <v>TransUnions Job Applicant Privacy Notice . What Well Bring: We are seeking a highly skilled Senior Full Stack Developer with 7-9 years of experience to join our engineering team | Expert-level proficiency in Java (Java 8+,Java 11 / 17 preferred) | 9 years of professional full stack development experience | 3+ years hands-on experience with Vue.js (Vue 2 /</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-12-29T20:39:26.441Z</v>
+        <v>2026-01-01T17:45:24.119Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1056,7 +1065,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-senior-net-developer-rudr-consultancy-services-udaipur-3-to-8-years-291225908518</v>
+        <v>https://www.naukri.com/job-listings-backend-ruby-stack-developer-xllent-corporate-services-pvt-ltd-bengaluru-1-to-6-years-311225909485</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1065,16 +1074,16 @@
         <v>Yes</v>
       </c>
       <c r="G9" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H9" t="str">
         <v>Yes</v>
       </c>
       <c r="I9" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J9" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K9" t="str">
         <v>Direct Apply</v>
@@ -1083,19 +1092,19 @@
         <v>Skipped</v>
       </c>
       <c r="M9" t="str">
-        <v>Senior .Net Developer</v>
+        <v>Backend Ruby Stack Developer</v>
       </c>
       <c r="N9" t="str">
-        <v>Leading Client</v>
+        <v>Xllent Corporate Services Pvt Ltd</v>
       </c>
       <c r="O9" t="str">
-        <v>3 - 8 years</v>
+        <v>1 - 6 years</v>
       </c>
       <c r="P9" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q9" t="str">
-        <v>Udaipur</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R9" t="str">
         <v>1 day ago</v>
@@ -1104,16 +1113,16 @@
         <v>1</v>
       </c>
       <c r="T9" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U9" t="str">
-        <v>jquery, asp.net, phonegap, javascript, web programming, css, c++, web services, ado.net, dbms, t-sql, ajax, sql, java, linux, json, html, mysql, data structures, mvc, wcf, c#, rest, python, c, vb, relational databases, sql server, angular, linq, web technologies, .net, angularjs</v>
+        <v>auditing, accounting, ruby, rails, design patterns, css, python, c++, bootstrap, ssl, javascript, jquery, sql, eclipse, notepad++, database management, react.js, git, java, design and coding, postgresql, jenkins, mysql</v>
       </c>
       <c r="V9" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W9" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Accounting / Auditing</v>
       </c>
       <c r="X9" t="str">
         <v>Full Time, Permanent</v>
@@ -1121,13 +1130,16 @@
       <c r="Y9" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Z9" t="str">
+        <v>2.3</v>
+      </c>
       <c r="AA9" t="str">
-        <v>B.Tech/BCA/MCA with 3-10 years experience in .NET technologies | Deliver solutions for large-scale enterprises using VB.NET/C#, SQL, and related web technologies | Salary is best in the industry</v>
+        <v>1 to 6 years of experience in Ruby stack development with a background in accounting and auditing | Develop and maintain backend systems, collaborate with teams, design database schemas, ensure code quality</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-12-29T20:39:31.540Z</v>
+        <v>2026-01-01T17:45:38.043Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1136,7 +1148,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-net-mvc-developer-cjk-knowledgeworks-work-from-office-kilpauk-knowledgeworks-global-kgl-chennai-3-to-7-years-240125009569</v>
+        <v>https://www.naukri.com/job-listings-java-python-developer-persistent-pune-3-to-6-years-311225022813</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1163,34 +1175,34 @@
         <v>Skipped</v>
       </c>
       <c r="M10" t="str">
-        <v>.NET &amp; MVC Developer - CJK KnowledgeWorks(Work from Office- Kilpauk)</v>
+        <v>Java Python Developer</v>
       </c>
       <c r="N10" t="str">
-        <v>KnowledgeWorks Global (KGL)</v>
+        <v>Persistent</v>
       </c>
       <c r="O10" t="str">
-        <v>3 - 7 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P10" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q10" t="str">
-        <v>Chennai( Kilpauk )</v>
+        <v>Pune</v>
       </c>
       <c r="R10" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S10" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T10" t="str">
-        <v>50+</v>
+        <v>100+</v>
       </c>
       <c r="U10" t="str">
-        <v>Net Mvc, asp.net, Asp.Net Core, MVC, MVC Architecture, .Net Core, SQL Server Development, .NET Compact Framework, MVC Framework, Asp.Net Web Api, Asp.Net Core Mvc, ASP.Net MVC, Angular, Fullstack Development, ASP.Net Ajax, .Net, Entity Framework</v>
+        <v>Java, Microservice, Spring boot, Python</v>
       </c>
       <c r="V10" t="str">
-        <v>Full Stack Developer</v>
+        <v>IT Infrastructure Services - Other</v>
       </c>
       <c r="W10" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1199,18 +1211,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y10" t="str">
-        <v>Software Development</v>
+        <v>IT Infrastructure Services</v>
       </c>
       <c r="Z10" t="str">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="AA10" t="str">
-        <v>Minimum 3 years experience in .Net with MVC framework, proficient in ASP.NET, C#, SQL Server, and Angular JS | Build and maintain .NET applications, ensure code quality, and provide technical support</v>
+        <v>3+ years of experience in full stack or back-end development with Java and Python | Develop and maintain applications using Java, Python, Spring Boot, and microservices | Competitive salary and benefits package with opportunities for growth and education</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-12-29T20:40:02.479Z</v>
+        <v>2026-01-01T17:45:51.770Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1219,7 +1231,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-291225921679</v>
+        <v>https://www.naukri.com/job-listings-backend-developer-java-codemind-staffing-solutions-chennai-3-to-5-years-311225911471</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1240,34 +1252,34 @@
         <v>Good Match</v>
       </c>
       <c r="K11" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L11" t="str">
         <v>Skipped</v>
       </c>
       <c r="M11" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Backend Developer - Java</v>
       </c>
       <c r="N11" t="str">
-        <v>Accenture</v>
+        <v>IT</v>
       </c>
       <c r="O11" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q11" t="str">
-        <v>Bengaluru</v>
+        <v>Chennai</v>
       </c>
       <c r="R11" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S11" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U11" t="str">
-        <v>software engineer, front end, kubernetes, api development, cloud services, restful, software development, version control, javascript, jquery, sql server, sql, docker, restful apis, git, devops, software solutions, mvc, agile, postgres</v>
+        <v>backend developer, rest, oracle, rdbms, tomcat, operating system, weblogic, hibernate, sql server, core java, sql, java, jboss, apis, mysql, java programming</v>
       </c>
       <c r="V11" t="str">
         <v>Full Stack Developer</v>
@@ -1281,16 +1293,13 @@
       <c r="Y11" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z11" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA11" t="str">
-        <v>Minimum 5 years of experience in DevOps with proficiency in cloud services and containerization technologies | Develop and maintain software solutions using C# and .NET Core, design RESTful APIs, and mentor junior team members</v>
+        <v>Bachelor's degree in Computer Science with 4-6 years of experience in Java and JEE stack, strong Object-Oriented programming skills | Develop and design code, mentor junior developers, create test-driven environments, and travel to customer locations as needed</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-12-29T20:40:07.217Z</v>
+        <v>2026-01-01T17:46:05.459Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1299,7 +1308,7 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-291225919029</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-311225920072</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
@@ -1332,25 +1341,25 @@
         <v>Accenture</v>
       </c>
       <c r="O12" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P12" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q12" t="str">
-        <v>Bengaluru</v>
+        <v>Pune</v>
       </c>
       <c r="R12" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S12" t="str">
-        <v>Less than 10</v>
+        <v>13</v>
       </c>
       <c r="U12" t="str">
-        <v>software engineer, front end, kubernetes, application developer, restful, react, sql server, sql, microservices, docker, angular, restful apis, git, devops, oops, kafka, jenkins, scrum, mvc, agile, aws, mongodb, architecture, azure</v>
+        <v>software engineer, css, full stack development, version control, hibernate, javascript, database management, java, git, postgresql, design, full stack, software solutions, mysql, web development, html, agile</v>
       </c>
       <c r="V12" t="str">
-        <v>Search Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W12" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1365,12 +1374,12 @@
         <v>3.7</v>
       </c>
       <c r="AA12" t="str">
-        <v>Minimum 3 years experience in ASP.NET MVC and strong understanding of .NET Core, Microservices, and RESTful APIs | Develop custom software solutions, engage in design and coding, participate in team discussions, and conduct code reviews</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in web technologies and backend frameworks | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-12-29T20:40:12.565Z</v>
+        <v>2026-01-01T17:46:10.329Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1379,13 +1388,13 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-291225921439</v>
+        <v>https://www.naukri.com/job-listings-intermediate-application-developer-java-ups-express-private-limited-chennai-3-to-7-years-311225917307</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
       </c>
       <c r="F13" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G13" t="str">
         <v>Yes</v>
@@ -1394,63 +1403,63 @@
         <v>Yes</v>
       </c>
       <c r="I13" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J13" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K13" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L13" t="str">
         <v>Skipped</v>
       </c>
       <c r="M13" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Intermediate Application Developer - JAVA</v>
       </c>
       <c r="N13" t="str">
-        <v>Accenture</v>
+        <v>UPS Supply Chain Solutions (UPS SCS)</v>
       </c>
       <c r="O13" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P13" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q13" t="str">
-        <v>Bengaluru</v>
+        <v>Chennai</v>
       </c>
       <c r="R13" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S13" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U13" t="str">
-        <v>software engineer, kubernetes, react, iac, microservices, docker, tensorflow, iam, devops, pytorch, debugging, mvc, graphql, architecture, azure, front end, python, ai, aws sagemaker, angular, kafka, full stack, terraform, agile, aws</v>
+        <v>application developer, project management, software development, sql server, sql, microservices, spring boot, software development lifecycle, java, git, linux, jenkins, agile methodologies, coaching, software engineering, agile, programming</v>
       </c>
       <c r="V13" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W13" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Courier / Logistics</v>
       </c>
       <c r="X13" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y13" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Z13" t="str">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="AA13" t="str">
-        <v>Bachelor's degree in computer science or related field; 5-12 years of full-stack development experience with strong proficiency in .NET and Python; familiarity with AI/ML integration and multi-cloud environments | Develop and deploy custom software solutions; lead AI-driven solution design; collaborate with teams for application development and integration</v>
+        <v>Bachelor's Degree in Computer Science or related field; experience with Java/J2EE, Spring, Microservices, SQL Server, and Cloud technology | Modernize legacy systems to Cloud applications; design, develop, maintain, and test software; provide project management and troubleshooting</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-12-29T20:40:17.268Z</v>
+        <v>2026-01-01T17:46:25.576Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1459,13 +1468,13 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-291225923684</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-311225919511</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
       </c>
       <c r="F14" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G14" t="str">
         <v>Yes</v>
@@ -1474,10 +1483,10 @@
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K14" t="str">
         <v>External Apply</v>
@@ -1498,7 +1507,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q14" t="str">
-        <v>Pune</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R14" t="str">
         <v>1 day ago</v>
@@ -1507,10 +1516,10 @@
         <v>Less than 10</v>
       </c>
       <c r="U14" t="str">
-        <v>software engineer, kubernetes, react, iac, microservices, docker, tensorflow, iam, devops, pytorch, debugging, mvc, graphql, architecture, azure, front end, python, ai, aws sagemaker, angular, kafka, full stack, terraform, agile, aws</v>
+        <v>software engineer, application developer, restful, sql, microservices, web development frameworks, database management, java, restful apis, git, microservices architecture, full stack, software solutions, web development, agile, architecture</v>
       </c>
       <c r="V14" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W14" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1519,18 +1528,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y14" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Z14" t="str">
         <v>3.7</v>
       </c>
       <c r="AA14" t="str">
-        <v>5+ years of experience in .NET Full Stack Development with strong skills in Python and front-end frameworks like React or Angular | Develop and enhance custom software solutions, lead AI-driven design, and implement multi-cloud applications</v>
+        <v>Minimum 5 years experience in Java Full Stack Development with proficiency in web development frameworks and SQL | Develop custom software solutions, collaborate with teams, and ensure timely delivery of projects</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-12-29T20:40:21.946Z</v>
+        <v>2026-01-01T17:46:30.270Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1539,7 +1548,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-2-to-5-years-291225925315</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-311225919514</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1548,16 +1557,16 @@
         <v>Yes</v>
       </c>
       <c r="G15" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H15" t="str">
         <v>Yes</v>
       </c>
       <c r="I15" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K15" t="str">
         <v>External Apply</v>
@@ -1578,16 +1587,16 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q15" t="str">
-        <v>Navi Mumbai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R15" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S15" t="str">
-        <v>Less than 10</v>
+        <v>35</v>
       </c>
       <c r="U15" t="str">
-        <v>software engineer, front end, application developer, css, full stack development, version control, business processes, user experience, javascript, sql server, sql, back end, git, full stack, software solutions, debugging, construction, html, agile</v>
+        <v>software engineer, front end, application developer, css, restful, hibernate, javascript, nosql, sql, microservices, back end, database management, java, restful apis, microservices architecture, full stack, agile, architecture, nosql databases</v>
       </c>
       <c r="V15" t="str">
         <v>Full Stack Developer</v>
@@ -1605,12 +1614,12 @@
         <v>3.7</v>
       </c>
       <c r="AA15" t="str">
-        <v>Minimum . 2 year(s) of experience is required. Educational Qualification : 15 years full time education. Summary :As an Application Developer,you will engage in the design,construction,and configuration of applications tailored to fulfill specific business processes and application requirements | Required active participation / contribution in team discussions</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end and back-end technologies | Develop custom software solutions, collaborate with teams, and ensure timely delivery of application features</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-12-29T20:40:26.683Z</v>
+        <v>2026-01-01T17:46:34.970Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1619,7 +1628,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-3-to-8-years-291225923728</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-311225919755</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1652,22 +1661,22 @@
         <v>Accenture</v>
       </c>
       <c r="O16" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P16" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q16" t="str">
-        <v>Pune</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R16" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S16" t="str">
-        <v>Less than 10</v>
+        <v>10</v>
       </c>
       <c r="U16" t="str">
-        <v>software engineer, restful, full stack development, version control, sql server, sql, web development frameworks, angular, database management, git, api design, full stack, agile methodologies, software solutions, debugging, web development, agile</v>
+        <v>software engineer, front end, application developer, css, version control, hibernate, javascript, nosql, sql, back end, database management, java, git, business process, full stack, software solutions, html, agile, nosql databases</v>
       </c>
       <c r="V16" t="str">
         <v>Full Stack Developer</v>
@@ -1685,12 +1694,12 @@
         <v>3.7</v>
       </c>
       <c r="AA16" t="str">
-        <v>Minimum 3 years experience in .Net Full Stack Development with proficiency in ASP.NET and Angular | Develop custom software solutions, collaborate with teams, and troubleshoot software issues</v>
+        <v>Minimum 5 years experience in Java Full Stack Development with proficiency in front-end technologies and back-end frameworks | Develop custom software solutions, collaborate with teams, and ensure timely delivery of application features</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-12-29T20:40:31.275Z</v>
+        <v>2026-01-01T17:46:39.738Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1699,7 +1708,7 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-2-to-5-years-291225924738</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-311225919487</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
@@ -1708,16 +1717,16 @@
         <v>Yes</v>
       </c>
       <c r="G17" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H17" t="str">
         <v>Yes</v>
       </c>
       <c r="I17" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J17" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K17" t="str">
         <v>External Apply</v>
@@ -1738,16 +1747,16 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q17" t="str">
-        <v>Navi Mumbai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R17" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S17" t="str">
-        <v>Less than 10</v>
+        <v>16</v>
       </c>
       <c r="U17" t="str">
-        <v>software engineer, front end, application developer, restful, web services, version control, react, sql server, sql, angular, database management, restful apis, git, business process, apis, full stack, software solutions, agile</v>
+        <v>software engineer, front end, application developer, css, version control, user experience, hibernate, javascript, nosql, sql, back end, database management, java, git, business process, full stack, software solutions, html, agile, nosql databases</v>
       </c>
       <c r="V17" t="str">
         <v>Full Stack Developer</v>
@@ -1765,12 +1774,12 @@
         <v>3.7</v>
       </c>
       <c r="AA17" t="str">
-        <v>Minimum . 2 year(s) of experience is required. Educational Qualification : 15 years full time education. Summary :As an Application Developer,you will design,build,and configure applications to meet business process and application requirements | A 15 years full time education is required. . Qualification 15 years full time education | Good To Have</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end technologies and back-end frameworks | Develop custom software solutions, collaborate with teams, and mentor junior members</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-12-29T20:40:36.010Z</v>
+        <v>2026-01-01T17:46:44.545Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1779,25 +1788,25 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-navi-mumbai-3-to-8-years-291225924406</v>
+        <v>https://www.naukri.com/job-listings-sse-specialist-software-engineer-java-dev-societe-generale-global-solution-centre-bengaluru-3-to-8-years-311225503775</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
       </c>
       <c r="F18" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G18" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H18" t="str">
         <v>Yes</v>
       </c>
       <c r="I18" t="str">
-        <v>2/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J18" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K18" t="str">
         <v>External Apply</v>
@@ -1806,10 +1815,10 @@
         <v>Skipped</v>
       </c>
       <c r="M18" t="str">
-        <v>Custom Software Engineer</v>
+        <v>SSE -Specialist Software Engineer (Java dev)</v>
       </c>
       <c r="N18" t="str">
-        <v>Accenture</v>
+        <v>Societe Generale Global Solution Centre</v>
       </c>
       <c r="O18" t="str">
         <v>3 - 8 years</v>
@@ -1818,16 +1827,19 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q18" t="str">
-        <v>Navi Mumbai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R18" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S18" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T18" t="str">
+        <v>50+</v>
       </c>
       <c r="U18" t="str">
-        <v>software engineer, front end, application developer, cloud services, restful, web services, business processes, react, sql server, sql, cloud, angular, database management, restful apis, business process, apis, full stack, construction</v>
+        <v>kubernetes, spring cloud, openshift, spring data, microservices, docker, spring, angular, spring boot, java, git, pair programming, spring security, spring integration, it projects, postgresql, microservices development, mysql, agile, web markup, communication skills</v>
       </c>
       <c r="V18" t="str">
         <v>Full Stack Developer</v>
@@ -1842,15 +1854,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z18" t="str">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="AA18" t="str">
-        <v/>
+        <v>Angular (v&gt;12) -&gt; this is a nice to have . Good knowledge of microservice development patterns . Good knowledge of microservice architectures . Good knowledge of Docker,Kubernetes or Openshift (v3 / 4) . | Required . | Profile required . Methodologies: Agile . Ability to work in a team,acting proactively .</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-12-29T20:40:40.696Z</v>
+        <v>2026-01-01T17:46:49.423Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1859,13 +1871,13 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-3-to-5-years-291225923238</v>
+        <v>https://www.naukri.com/job-listings-returnship-opportunity-java-angular-fullstack-developer-ups-express-private-limited-chennai-2-to-7-years-311225917038</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
       </c>
       <c r="F19" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G19" t="str">
         <v>Yes</v>
@@ -1874,63 +1886,63 @@
         <v>Yes</v>
       </c>
       <c r="I19" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J19" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K19" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L19" t="str">
         <v>Skipped</v>
       </c>
       <c r="M19" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Returnship Opportunity - Java / Angular(Fullstack) - Developer</v>
       </c>
       <c r="N19" t="str">
-        <v>Accenture</v>
+        <v>UPS Supply Chain Solutions (UPS SCS)</v>
       </c>
       <c r="O19" t="str">
-        <v>3 - 5 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P19" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q19" t="str">
-        <v>Pune</v>
+        <v>Chennai</v>
       </c>
       <c r="R19" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S19" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U19" t="str">
-        <v>software engineer, front end, kubernetes, python, predictive analytics, ai, react, devops engineer, microservices, docker, angular, iam, spark, compliance, kafka, full stack, mvc, hadoop, graphql, big data, aws, architecture, azure</v>
+        <v>java, tfs, front end, security compliance, restful, mathematics, jsp, javascript, angular, git, apis, grafana, compliance, devops, design, jenkins, debugging, scrum, html, agile, maintenance, azure, statistics, communication skills</v>
       </c>
       <c r="V19" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W19" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Courier / Logistics</v>
       </c>
       <c r="X19" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y19" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Z19" t="str">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="AA19" t="str">
-        <v>12 to 20+ years in enterprise architecture with strong .NET Core, Python, and AI integration skills | Design and implement application-heavy enterprise architectures across multi-cloud environments</v>
+        <v>2 years of experience in Java and Angular development; Bachelor's degree in Computer Science or related field | Support full systems life cycle management; Collaborate with teams for effective communication; Maintain and develop applications</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-12-29T20:40:45.777Z</v>
+        <v>2026-01-01T17:47:03.154Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1939,7 +1951,7 @@
         <v>19/20</v>
       </c>
       <c r="D20" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-5-years-291225921956</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-311225920285</v>
       </c>
       <c r="E20" t="str">
         <v>Yes</v>
@@ -1972,25 +1984,25 @@
         <v>Accenture</v>
       </c>
       <c r="O20" t="str">
-        <v>3 - 5 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P20" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q20" t="str">
-        <v>Bengaluru</v>
+        <v>Pune</v>
       </c>
       <c r="R20" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S20" t="str">
-        <v>Less than 10</v>
+        <v>14</v>
       </c>
       <c r="U20" t="str">
-        <v>software engineer, front end, kubernetes, python, predictive analytics, ai, react, devops engineer, microservices, docker, angular, iam, spark, compliance, kafka, full stack, mvc, hadoop, graphql, big data, aws, architecture, azure</v>
+        <v>software engineer, snowflake, data warehouse, python, scala, airflow, database technologies, cloud platforms, elt, data engineering, sql, etl pipelines, java, git, software solutions, agile, aws, etl, programming, architecture, azure</v>
       </c>
       <c r="V20" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Data Platform Engineer</v>
       </c>
       <c r="W20" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1999,18 +2011,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y20" t="str">
-        <v>Quality Assurance and Testing</v>
+        <v>Software Development</v>
       </c>
       <c r="Z20" t="str">
         <v>3.7</v>
       </c>
       <c r="AA20" t="str">
-        <v>12 to 20+ years in enterprise architecture with strong .NET Core, Python, and AI integration skills | Design and implement application-heavy enterprise architectures across multi-cloud environments, lead full-stack development, and ensure seamless system integrations</v>
+        <v>Minimum 5 years of experience in Data Engineering; proficiency in Data Engineering and Snowflake; strong programming skills in Python, Java, or Scala | Develop custom software solutions; manage team decisions; analyze project requirements and translate them into technical specifications</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-12-29T20:40:50.483Z</v>
+        <v>2026-01-01T17:47:08.545Z</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2019,13 +2031,13 @@
         <v>20/20</v>
       </c>
       <c r="D21" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-291225923006</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-mumbai-3-to-8-years-311225920122</v>
       </c>
       <c r="E21" t="str">
         <v>Yes</v>
       </c>
       <c r="F21" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G21" t="str">
         <v>Yes</v>
@@ -2034,10 +2046,10 @@
         <v>Yes</v>
       </c>
       <c r="I21" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J21" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K21" t="str">
         <v>External Apply</v>
@@ -2052,22 +2064,22 @@
         <v>Accenture</v>
       </c>
       <c r="O21" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P21" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q21" t="str">
-        <v>Pune</v>
+        <v>Mumbai</v>
       </c>
       <c r="R21" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S21" t="str">
-        <v>Less than 10</v>
+        <v>17</v>
       </c>
       <c r="U21" t="str">
-        <v>software engineer, rest, software development, web services, microsoft dynamics, user experience, javascript, sql server, sales, sql, marketing, active directory, software solutions, http, agile, ssis, dynamics 365, soap, architecture, azure, crm</v>
+        <v>software engineer, front end, css, software development, business processes, front end technologies, javascript, sql, application development, angular, database management, java, software solutions, debugging, scrum, construction, html, agile</v>
       </c>
       <c r="V21" t="str">
         <v>Full Stack Developer</v>
@@ -2085,7 +2097,7 @@
         <v>3.7</v>
       </c>
       <c r="AA21" t="str">
-        <v>Minimum 5 years experience in Microsoft Dynamics CRM Technical and 15 years full-time education | Develop and customize Microsoft Dynamics 365 applications, manage timelines, and ensure quality</v>
+        <v>Minimum 3 years experience in Java and 1 year in Microsoft ASP.NET; proficiency in Java, JavaScript, Angular, and SQL | Develop custom software solutions, collaborate with teams, and participate in code reviews</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the issue of savaing status of job
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-03T13:43:37.265Z</v>
+        <v>2026-01-04T10:28:02.489Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -496,13 +496,13 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-t-systems-ict-india-pvt-ltd-pune-bengaluru-1-to-3-years-020126023473</v>
+        <v>https://www.naukri.com/job-listings-software-developer-actionbeans-software-hyderabad-delhi-ncr-mumbai-all-areas-0-to-3-years-030126012865</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
       </c>
       <c r="F2" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G2" t="str">
         <v>Yes</v>
@@ -511,7 +511,7 @@
         <v>No</v>
       </c>
       <c r="I2" t="str">
-        <v>3/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J2" t="str">
         <v>Poor Match</v>
@@ -523,34 +523,34 @@
         <v>Skipped</v>
       </c>
       <c r="M2" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Software Developer</v>
       </c>
       <c r="N2" t="str">
-        <v>T-Systems ICT India Pvt Ltd</v>
+        <v>Actionbeans Software</v>
       </c>
       <c r="O2" t="str">
-        <v>1 - 3 years</v>
+        <v>0 - 3 years</v>
       </c>
       <c r="P2" t="str">
-        <v>Not Disclosed</v>
+        <v>3-4.25 Lacs P.A.</v>
       </c>
       <c r="Q2" t="str">
-        <v>Pune</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R2" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S2" t="str">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T2" t="str">
         <v>100+</v>
       </c>
       <c r="U2" t="str">
-        <v>Java, Typescript, Javascript, Full Stack, Spring Boot, React, Angular</v>
+        <v>SQL, C#, Java, Javascript, .Net, HTML, Python</v>
       </c>
       <c r="V2" t="str">
-        <v>Technical Consultant</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W2" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -559,18 +559,15 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y2" t="str">
-        <v>IT Consulting</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>3.8</v>
+        <v>Software Development</v>
       </c>
       <c r="AA2" t="str">
-        <v>1-3 years experience in web application development with strong expertise in JavaScript, AngularJS, or NodeJS | Design, develop, and maintain web applications; implement RESTful Web Services and Microservices; write SQL queries; develop PERL and SHELL scripts; troubleshoot and collaborate using Agile Scrum</v>
+        <v>Motivated Full-Stack Developer with experience in C#, Java, JavaScript, .Net, HTML, Python, and SQL | Build and take ownership of features end-to-end in real production systems</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-03T13:43:42.719Z</v>
+        <v>2026-01-04T10:28:07.625Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -579,7 +576,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-9267977094-mobile-user-new-delhi-2-to-6-years-030126012931</v>
+        <v>https://www.naukri.com/job-listings-fullstack-python-developer-r2r-consults-mumbai-suburban-navi-mumbai-mumbai-all-areas-3-to-5-years-161225020280</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -588,16 +585,16 @@
         <v>Yes</v>
       </c>
       <c r="G3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H3" t="str">
         <v>Yes</v>
       </c>
       <c r="I3" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J3" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K3" t="str">
         <v>Direct Apply</v>
@@ -606,37 +603,37 @@
         <v>Skipped</v>
       </c>
       <c r="M3" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Fullstack Python Developer</v>
       </c>
       <c r="N3" t="str">
-        <v>9267977094 Mobile User</v>
+        <v>R2R Consults</v>
       </c>
       <c r="O3" t="str">
-        <v>2 - 6 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="P3" t="str">
-        <v>3.36-3.6 Lacs P.A.</v>
+        <v>8-10 Lacs P.A.</v>
       </c>
       <c r="Q3" t="str">
-        <v>New Delhi( Delhi Cantonment )</v>
+        <v>Mumbai Suburban</v>
       </c>
       <c r="R3" t="str">
-        <v>Few hours ago</v>
+        <v>1 day ago</v>
       </c>
       <c r="S3" t="str">
         <v>1</v>
       </c>
       <c r="T3" t="str">
-        <v>50+</v>
+        <v>100+</v>
       </c>
       <c r="U3" t="str">
-        <v>Java Fullstack, Java, Spring Boot, Spring, Microservices</v>
+        <v>React.Js, Python, Typescript, Django, Postgresql, MySQL, Javascript, Flask</v>
       </c>
       <c r="V3" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W3" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Advertising &amp; Marketing</v>
       </c>
       <c r="X3" t="str">
         <v>Full Time, Permanent</v>
@@ -645,12 +642,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA3" t="str">
-        <v>Experience in Java, Spring Boot, and Microservices | Design, develop, test, and maintain full-stack applications; collaborate with cross-functional teams | Health insurance and provident fund provided</v>
+        <v>3 to 5 years of experience in Full Stack Development with strong skills in React.js and Python | Develop responsive UIs, build backend services, and maintain RESTful APIs</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2026-01-03T13:44:14.749Z</v>
+        <v>2026-01-04T10:28:12.764Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -659,7 +656,7 @@
         <v>3/20</v>
       </c>
       <c r="D4" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-apexon-bengaluru-3-to-8-years-020126021512</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-location-pune-zycus-infotech-pune-2-to-6-years-241125016928</v>
       </c>
       <c r="E4" t="str">
         <v>Yes</v>
@@ -680,37 +677,37 @@
         <v>Good Match</v>
       </c>
       <c r="K4" t="str">
-        <v>Direct Apply</v>
+        <v>No Apply Button</v>
       </c>
       <c r="L4" t="str">
         <v>Skipped</v>
       </c>
       <c r="M4" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Java Full Stack Developer (Location: Pune)</v>
       </c>
       <c r="N4" t="str">
-        <v>Apexon</v>
+        <v>Zycus Infotech</v>
       </c>
       <c r="O4" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 6 years</v>
       </c>
       <c r="P4" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q4" t="str">
-        <v>Bengaluru</v>
+        <v>Pune</v>
       </c>
       <c r="R4" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S4" t="str">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T4" t="str">
         <v>100+</v>
       </c>
       <c r="U4" t="str">
-        <v>Java, Java Spring Boot, React.Js, Javascript, Spring Boot, HTML, Java Fullstack, AWS</v>
+        <v>Generative Ai, Java Spring Boot, Java Fullstack, React.Js, Microservices, Angularjs, Java, Artificial Intelligence, Full Stack, Spring Boot</v>
       </c>
       <c r="V4" t="str">
         <v>Full Stack Developer</v>
@@ -725,15 +722,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z4" t="str">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="AA4" t="str">
-        <v>Strong Java fundamentals, experience with Spring/Spring Boot, solid hands-on experience with React | Develop and maintain applications using Java, Spring, and React; work with RESTful services and databases</v>
+        <v>2+ years of Java development experience with strong proficiency in Spring Framework and Microservices architecture | Design, develop, and deploy Java-based backend services; develop front-end interfaces using Angular or React; integrate systems and collaborate in Agile environment | Competitive compensation and opportunities for career advancement</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2026-01-03T13:44:28.525Z</v>
+        <v>2026-01-04T10:28:17.883Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -742,25 +739,25 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-java-developer-srs-infoway-hyderabad-3-to-5-years-020126916175</v>
+        <v>https://www.naukri.com/job-listings-build-engineer-spire-technologies-and-solutions-bengaluru-1-to-3-years-020126007100</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
       </c>
       <c r="F5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G5" t="str">
         <v>Yes</v>
       </c>
       <c r="H5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I5" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J5" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K5" t="str">
         <v>Direct Apply</v>
@@ -769,51 +766,54 @@
         <v>Skipped</v>
       </c>
       <c r="M5" t="str">
-        <v>Full Stack Java Developer</v>
+        <v>Build Engineer</v>
       </c>
       <c r="N5" t="str">
-        <v>SRSInfoway</v>
+        <v>Spire Technologies And Solutions</v>
       </c>
       <c r="O5" t="str">
-        <v>3 - 5 years</v>
+        <v>1 - 3 years</v>
       </c>
       <c r="P5" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q5" t="str">
-        <v>Hyderabad</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R5" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S5" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T5" t="str">
         <v>100+</v>
       </c>
       <c r="U5" t="str">
-        <v>Java, Spring Boot, HTML5, Spring Security, JPA/Hibernate, Azure, or Google Cloud Platforms, Scrum/Kanban, openshift, CSS3, Jenkins, GitHub Actions, Git, JUnit, Mockito, AciveMQ, IBMMQ, Selenium, or Azure DevOps, Spring Batch, AWS, Kubernetes</v>
+        <v>Java / Spring Boot, Python Development, Build &amp; Configuration Management</v>
       </c>
       <c r="V5" t="str">
-        <v>Other</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W5" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Software Product</v>
       </c>
       <c r="X5" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y5" t="str">
-        <v>Other</v>
+        <v>Software Development</v>
+      </c>
+      <c r="Z5" t="str">
+        <v>3.5</v>
       </c>
       <c r="AA5" t="str">
-        <v>3-5 years of experience in full-stack development with strong skills in Java, Spring Boot, and cloud platforms | Design, develop, and maintain full-stack applications; implement security and batch processing; deploy and manage applications using Docker and Kubernetes</v>
+        <v>Proficient in Python, Java, JavaScript, ETL, and Microservices | Develop and maintain backend services, manage data processing and validation, and provide technical support</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2026-01-03T13:44:42.444Z</v>
+        <v>2026-01-04T10:28:22.720Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -822,25 +822,25 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-tata-consultancy-services-hyderabad-chennai-bengaluru-3-to-8-years-020126003483</v>
+        <v>https://www.naukri.com/job-listings-mobile-application-developer-exaflair-technologies-mohali-chandigarh-zirakpur-1-to-3-years-030126015753</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
       </c>
       <c r="F6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I6" t="str">
-        <v>4/undefined</v>
+        <v>1/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K6" t="str">
         <v>Direct Apply</v>
@@ -849,19 +849,19 @@
         <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Mobile Application Developer</v>
       </c>
       <c r="N6" t="str">
-        <v>Tata Consultancy Services</v>
+        <v>Exaflair Technologies</v>
       </c>
       <c r="O6" t="str">
-        <v>3 - 8 years</v>
+        <v>1 - 3 years</v>
       </c>
       <c r="P6" t="str">
-        <v>Not Disclosed</v>
+        <v>4-6 Lacs P.A.</v>
       </c>
       <c r="Q6" t="str">
-        <v>Chennai</v>
+        <v>Mohali</v>
       </c>
       <c r="R6" t="str">
         <v>1 day ago</v>
@@ -870,13 +870,13 @@
         <v>1</v>
       </c>
       <c r="T6" t="str">
-        <v>100+</v>
+        <v>33</v>
       </c>
       <c r="U6" t="str">
-        <v>Java, React.Js, Java Spring Boot</v>
+        <v>Flutter, React Native, Expo, IOS, XCode, Android</v>
       </c>
       <c r="V6" t="str">
-        <v>Full Stack Developer</v>
+        <v>Application Engineer</v>
       </c>
       <c r="W6" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -885,18 +885,15 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y6" t="str">
-        <v>Software Development</v>
-      </c>
-      <c r="Z6" t="str">
-        <v>3.3</v>
+        <v>Engineering</v>
       </c>
       <c r="AA6" t="str">
-        <v>Strong hands-on experience in Core Java, Hibernate, and XML technologies; knowledge of various file formats and SQL queries | Develop and maintain applications using Java, Hibernate, and Web services; handle data conversions and file formats</v>
+        <v>Bachelor's degree in Computer Science or related field; 1-3 years of experience in mobile development with React Native or Flutter; strong hands-on experience with JavaScript/TypeScript | Build, test, and deploy high-quality mobile apps for iOS and Android; manage app submissions and updates; take ownership of the full development cycle | Competitive compensation based on experience and impact</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2026-01-03T13:45:21.037Z</v>
+        <v>2026-01-04T10:28:27.840Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -905,13 +902,13 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-full-stack-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-020126919921</v>
+        <v>https://www.naukri.com/job-listings-senior-software-engineer-matrecomm-technologies-bengaluru-3-to-7-years-030126015917</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
       </c>
       <c r="F7" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G7" t="str">
         <v>Yes</v>
@@ -920,28 +917,28 @@
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K7" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L7" t="str">
         <v>Skipped</v>
       </c>
       <c r="M7" t="str">
-        <v>Full Stack Engineer</v>
+        <v>Senior Software Engineer</v>
       </c>
       <c r="N7" t="str">
-        <v>Accenture</v>
+        <v>Matrecomm Technologies</v>
       </c>
       <c r="O7" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P7" t="str">
-        <v>Not Disclosed</v>
+        <v>8-14 Lacs P.A.</v>
       </c>
       <c r="Q7" t="str">
         <v>Bengaluru</v>
@@ -950,19 +947,19 @@
         <v>1 day ago</v>
       </c>
       <c r="S7" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T7" t="str">
-        <v>50</v>
+        <v>100+</v>
       </c>
       <c r="U7" t="str">
-        <v>css, java, html, javascript, spring boot, continuous integration, kubernetes, ci/cd, vue.js, ajax, docker, sql, spring, react.js, git, postgresql, gcp, devops, ATCI-5092539-S1904794, jenkins, debugging, typescript, mongodb, rest, rdbms, microsoft azure, nosql, angular, full stack, agile, aws</v>
+        <v>Technical Architecture, C++, Networking, React.Js</v>
       </c>
       <c r="V7" t="str">
-        <v>Search Engineer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W7" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Software Product</v>
       </c>
       <c r="X7" t="str">
         <v>Full Time, Permanent</v>
@@ -971,15 +968,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z7" t="str">
-        <v>3.7</v>
+        <v>3.0</v>
       </c>
       <c r="AA7" t="str">
-        <v>Minimum 5 years experience in Java Full Stack Development with strong proficiency in Java 8+, Spring Boot, and RESTful web services | Develop and maintain server-side logic, create RESTful APIs, and build responsive web user interfaces</v>
+        <v>Bachelor's or Master's in Computer Science or Engineering; strong proficiency in C++, ReactJS/NextJS, and networking protocols; experience in NMS software development | Design and develop high-performance C++ applications and web-based UI applications; implement features for Network Management Systems; ensure code quality and mentor junior engineers | Competitive compensation and growth opportunities</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2026-01-03T13:45:26.830Z</v>
+        <v>2026-01-04T10:28:32.713Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -988,7 +985,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-java-developer-3-8-yrs-ra-infosys-infosys-hyderabad-pune-bengaluru-3-to-8-years-270525024163</v>
+        <v>https://www.naukri.com/job-listings-fullstack-developer-net-core-angular-cydez-technology-consulting-services-kochi-3-to-6-years-271125032503</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -997,16 +994,16 @@
         <v>Yes</v>
       </c>
       <c r="G8" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H8" t="str">
         <v>Yes</v>
       </c>
       <c r="I8" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J8" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K8" t="str">
         <v>Direct Apply</v>
@@ -1015,31 +1012,31 @@
         <v>Skipped</v>
       </c>
       <c r="M8" t="str">
-        <v>Java Developer -(3-8 yrs)-RA @Infosys</v>
+        <v>Fullstack Developer(.NET Core +Angular)</v>
       </c>
       <c r="N8" t="str">
-        <v>Infosys</v>
+        <v>Cydez Technology Consulting Services</v>
       </c>
       <c r="O8" t="str">
-        <v>3 - 8 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P8" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q8" t="str">
-        <v>Pune</v>
+        <v>Kochi</v>
       </c>
       <c r="R8" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S8" t="str">
-        <v>9999</v>
+        <v>10</v>
       </c>
       <c r="T8" t="str">
-        <v>100+</v>
+        <v>47</v>
       </c>
       <c r="U8" t="str">
-        <v>Java, Hibernate, Spring Boot, Microservices</v>
+        <v>.Net Core, Angular, SQL, .Net, CSS, scss, sql constraints, rsjs operators, Html/Css, Javascript, method overriding, Exception Handling, API, dependency injuction</v>
       </c>
       <c r="V8" t="str">
         <v>Full Stack Developer</v>
@@ -1054,15 +1051,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z8" t="str">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="AA8" t="str">
-        <v>3 to 8 years of experience in Java, Spring Boot, and Hibernate; Btech/BE, Mtech/ME, BCA/MCA, BSC/MSC preferred | Develop and maintain Java applications using Spring Boot and Hibernate</v>
+        <v>3+ years of .NET development experience and strong proficiency in Angular | Develop, test, and maintain web applications; collaborate with teams to deliver features; troubleshoot and upgrade applications</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2026-01-03T13:45:40.978Z</v>
+        <v>2026-01-04T10:28:37.856Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1071,7 +1068,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-location-pune-zycus-infotech-pune-2-to-6-years-241125016928</v>
+        <v>https://www.naukri.com/job-listings-senior-engineer-angularjs-nagarro-mumbai-all-areas-3-to-5-years-030126010218</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1080,52 +1077,52 @@
         <v>Yes</v>
       </c>
       <c r="G9" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H9" t="str">
         <v>Yes</v>
       </c>
       <c r="I9" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J9" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K9" t="str">
-        <v>No Apply Button</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L9" t="str">
         <v>Skipped</v>
       </c>
       <c r="M9" t="str">
-        <v>Java Full Stack Developer (Location: Pune)</v>
+        <v>Senior Engineer (Angularjs)</v>
       </c>
       <c r="N9" t="str">
-        <v>Zycus Infotech</v>
+        <v>Nagarro</v>
       </c>
       <c r="O9" t="str">
-        <v>2 - 6 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="P9" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q9" t="str">
-        <v>Pune</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R9" t="str">
-        <v>Few hours ago</v>
+        <v>1 day ago</v>
       </c>
       <c r="S9" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T9" t="str">
         <v>100+</v>
       </c>
       <c r="U9" t="str">
-        <v>Generative Ai, Java Spring Boot, Java Fullstack, React.Js, Microservices, Angularjs, Java, Artificial Intelligence, Full Stack, Spring Boot</v>
+        <v>CSS, HTML5, JavaScript, Angular</v>
       </c>
       <c r="V9" t="str">
-        <v>Full Stack Developer</v>
+        <v>Front End Developer</v>
       </c>
       <c r="W9" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1137,15 +1134,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z9" t="str">
-        <v>2.7</v>
+        <v>3.9</v>
       </c>
       <c r="AA9" t="str">
-        <v>2+ years of Java development experience with strong proficiency in Spring Framework and Microservices architecture | Design, develop, and deploy Java-based backend services; develop front-end interfaces using Angular or React; integrate systems and collaborate in Agile environment | Competitive compensation and opportunities for career advancement</v>
+        <v>Hands-on experience in UI development with Angular 8/10, HTML5, Typescript, and TDD | Write and review quality code, convert business requirements into technical designs, and define project guidelines</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2026-01-03T13:45:45.655Z</v>
+        <v>2026-01-04T10:28:42.719Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1154,7 +1151,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126919917</v>
+        <v>https://www.naukri.com/job-listings-hiring-php-developer-3-4years-exp-immediate-joiners-preferred-tya-business-solutions-bengaluru-3-to-4-years-290925027979</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1175,25 +1172,25 @@
         <v>Good Match</v>
       </c>
       <c r="K10" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L10" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M10" t="str">
-        <v>Application Developer</v>
+        <v>Hiring PHP Developer(3-4years Exp) Immediate Joiners Preferred</v>
       </c>
       <c r="N10" t="str">
-        <v>Accenture</v>
+        <v>TYA Business Solutions</v>
       </c>
       <c r="O10" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 4 years</v>
       </c>
       <c r="P10" t="str">
-        <v>Not Disclosed</v>
+        <v>10-15 Lacs P.A.</v>
       </c>
       <c r="Q10" t="str">
-        <v>Chennai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R10" t="str">
         <v>1 day ago</v>
@@ -1202,16 +1199,16 @@
         <v>1</v>
       </c>
       <c r="T10" t="str">
-        <v>13</v>
+        <v>50+</v>
       </c>
       <c r="U10" t="str">
-        <v>java, cloud services, application development, full stack, web application framework, css, jsp, jdbc, hibernate, jquery, microservices, sql, spring, database management, react.js, spring mvc, j2ee, json, web development, html, mysql, rest, javascript, spring boot, angular</v>
+        <v>HTML, Python, Artificial Intelligence, Problem Solving, Api Integration, Machine Learning, Laravel, Angular, Codeigniter, SQL, MySQL, PHP, api, AWS</v>
       </c>
       <c r="V10" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W10" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Accounting / Auditing</v>
       </c>
       <c r="X10" t="str">
         <v>Full Time, Permanent</v>
@@ -1220,15 +1217,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z10" t="str">
-        <v>3.7</v>
+        <v>3.0</v>
       </c>
       <c r="AA10" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in web development frameworks | Design, build, and configure applications; collaborate with teams; monitor project progress</v>
+        <v>3-4 years of experience as a Full Stack Developer with strong knowledge of Angular, PHP, and Python | Design and maintain scalable web applications, collaborate on technical solutions, and implement AI/ML projects | Direct mentorship from Tech Head and Founders, exposure to cutting-edge technologies</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2026-01-03T13:45:52.204Z</v>
+        <v>2026-01-04T10:29:15.660Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1237,7 +1234,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126919966</v>
+        <v>https://www.naukri.com/job-listings-react-native-js-developer-radius-infotech-noida-1-to-5-years-131125023303</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1258,37 +1255,37 @@
         <v>Good Match</v>
       </c>
       <c r="K11" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L11" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M11" t="str">
-        <v>Application Developer</v>
+        <v>React Native/JS Developer</v>
       </c>
       <c r="N11" t="str">
-        <v>Accenture</v>
+        <v>Radius Infotech</v>
       </c>
       <c r="O11" t="str">
-        <v>2 - 5 years</v>
+        <v>1 - 5 years</v>
       </c>
       <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q11" t="str">
-        <v>Chennai</v>
+        <v>Noida( Noida Extension )</v>
       </c>
       <c r="R11" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S11" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T11" t="str">
-        <v>26</v>
+        <v>100+</v>
       </c>
       <c r="U11" t="str">
-        <v>web application architecture, spring boot, java, design patterns, full stack, rest, css, version control, jsp, hibernate, ATCI-5152758-S1901091, javascript, jquery, sql, java standard edition, application development, spring, react.js, angular, git, spring mvc, j2ee, html, mysql</v>
+        <v>Native, React.Js, Development, IOS, Android</v>
       </c>
       <c r="V11" t="str">
         <v>Full Stack Developer</v>
@@ -1303,15 +1300,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z11" t="str">
-        <v>3.7</v>
+        <v>4.1</v>
       </c>
       <c r="AA11" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development and 15 years of full-time education | Design, build, and configure applications; engage in team discussions and code reviews</v>
+        <v>3-5 years of experience in front-end development with React Native &amp; React JS; strong proficiency in JavaScript (ES6+) and TypeScript | Build pixel-perfect UIs for mobile/web platforms; utilize animations for user experience; participate in agile sprints</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2026-01-03T13:45:56.899Z</v>
+        <v>2026-01-04T10:29:47.323Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1320,13 +1317,13 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-020126911923</v>
+        <v>https://www.naukri.com/job-listings-vms-executive-roadvision-ai-new-delhi-2-to-7-years-030126015470</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
       </c>
       <c r="F12" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G12" t="str">
         <v>Yes</v>
@@ -1335,40 +1332,43 @@
         <v>Yes</v>
       </c>
       <c r="I12" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J12" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K12" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L12" t="str">
         <v>Skipped</v>
       </c>
       <c r="M12" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Vms Executive</v>
       </c>
       <c r="N12" t="str">
-        <v>Accenture</v>
+        <v>Roadvision Ai</v>
       </c>
       <c r="O12" t="str">
-        <v>2 - 5 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P12" t="str">
-        <v>Not Disclosed</v>
+        <v>7.2-9.6 Lacs P.A.</v>
       </c>
       <c r="Q12" t="str">
-        <v>Bengaluru</v>
+        <v>New Delhi( Bhikaji Cama Place )</v>
       </c>
       <c r="R12" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S12" t="str">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="T12" t="str">
+        <v>42</v>
       </c>
       <c r="U12" t="str">
-        <v>software engineer, css, full stack development, version control, hibernate, javascript, database management, java, git, postgresql, design, full stack, software solutions, mysql, web development, html, agile</v>
+        <v>VMS, Java, DVR, C++, Linux, Cloud Services, Node.Js, Nvr, Computer Vision, Python</v>
       </c>
       <c r="V12" t="str">
         <v>Full Stack Developer</v>
@@ -1383,15 +1383,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z12" t="str">
-        <v>3.7</v>
+        <v>4.4</v>
       </c>
       <c r="AA12" t="str">
-        <v>Minimum 2 years experience in Java Full Stack Development with proficiency in web technologies and backend frameworks | Develop custom software solutions, collaborate with teams, and troubleshoot software issues</v>
+        <v>Experience in managing VMS infrastructure with Linux, Python, and Java; skilled in developing computer vision applications using Node.js and Cloud Services | Manage VMS infrastructure, develop computer vision applications, and collaborate on NVR/DVR integration projects</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2026-01-03T13:46:01.939Z</v>
+        <v>2026-01-04T10:29:52.176Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1400,7 +1400,7 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-python-angular-developer-net-connect-chennai-bengaluru-mumbai-all-areas-3-to-6-years-020126020126</v>
+        <v>https://www.naukri.com/job-listings-react-native-developer-primotech-technologies-mohali-3-to-5-years-030126016435</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
@@ -1409,16 +1409,16 @@
         <v>Yes</v>
       </c>
       <c r="G13" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H13" t="str">
         <v>Yes</v>
       </c>
       <c r="I13" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J13" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K13" t="str">
         <v>Direct Apply</v>
@@ -1427,34 +1427,31 @@
         <v>Skipped</v>
       </c>
       <c r="M13" t="str">
-        <v>Python Angular Developer</v>
+        <v>React Native Developer</v>
       </c>
       <c r="N13" t="str">
-        <v>Net Connect</v>
+        <v>Primotech Technologies</v>
       </c>
       <c r="O13" t="str">
-        <v>3 - 6 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="P13" t="str">
-        <v>6-12 Lacs P.A.</v>
+        <v>3-5 Lacs P.A.</v>
       </c>
       <c r="Q13" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Mohali</v>
       </c>
       <c r="R13" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S13" t="str">
-        <v>10</v>
-      </c>
-      <c r="T13" t="str">
-        <v>100+</v>
+        <v>31</v>
       </c>
       <c r="U13" t="str">
-        <v>Angular Development, Javascript, Angular, SQL, Python, Typescript, Node.Js, AWS</v>
+        <v>React Native, CLI, Expo, Typescript, Redux, React Native Js</v>
       </c>
       <c r="V13" t="str">
-        <v>Full Stack Developer</v>
+        <v>Front End Developer</v>
       </c>
       <c r="W13" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1465,16 +1462,13 @@
       <c r="Y13" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z13" t="str">
-        <v>3.1</v>
-      </c>
       <c r="AA13" t="str">
-        <v>Bachelor’s degree in Computer Science or related field; 3-6 years of full stack development experience; strong skills in Python (Flask/FastAPI) and Angular | Develop and maintain Python backend services; build scalable RESTful APIs; create responsive frontend applications using Angular | CTC ₹5 - 12 LPA</v>
+        <v>Skilled React Native Developer with strong experience in mobile app development and proficiency in Expo | Develop and optimize mobile applications using React Native and Expo, integrate Firebase services, and collaborate with UI/UX designers</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2026-01-03T13:46:15.670Z</v>
+        <v>2026-01-04T10:29:57.006Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1483,13 +1477,13 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126920028</v>
+        <v>https://www.naukri.com/job-listings-team-member-land-estate-adani-group-ahmedabad-0-to-4-years-030126011135</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
       </c>
       <c r="F14" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G14" t="str">
         <v>Yes</v>
@@ -1498,46 +1492,43 @@
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K14" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L14" t="str">
         <v>Skipped</v>
       </c>
       <c r="M14" t="str">
-        <v>Application Developer</v>
+        <v>Team Member - Land &amp; Estate</v>
       </c>
       <c r="N14" t="str">
-        <v>Accenture</v>
+        <v>Adani Group</v>
       </c>
       <c r="O14" t="str">
-        <v>2 - 5 years</v>
+        <v>0 - 4 years</v>
       </c>
       <c r="P14" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q14" t="str">
-        <v>Chennai</v>
+        <v>Ahmedabad</v>
       </c>
       <c r="R14" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S14" t="str">
-        <v>1</v>
-      </c>
-      <c r="T14" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U14" t="str">
-        <v>html, events, asynchronous apex, javascript, node, css, web services, hibernate, jquery, microservices, sql, spring, git, java, asp.net, j2ee, mongodb, ATCI-5153532-S1900788, c#, rest, version control, application development, spring boot, angular, node.js, javascript frameworks, angularjs</v>
+        <v>data management, data, arcgis, analytical, arcgis server, arc map, esri, dashboards, sql, gis, arcgis desktop, arcgis enterprise, postgresql, html, c#, python, workflow, remote sensing, analysis, machine learning, javascript, sql server, geographical information system, survey, .net, data entry</v>
       </c>
       <c r="V14" t="str">
-        <v>Full Stack Developer</v>
+        <v>Data Science &amp; Analytics - Other</v>
       </c>
       <c r="W14" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1546,18 +1537,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y14" t="str">
-        <v>Software Development</v>
+        <v>Data Science &amp; Analytics - Other</v>
       </c>
       <c r="Z14" t="str">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="AA14" t="str">
-        <v>Minimum 3 years experience in Node.js and 15 years full-time education | Design, build, and configure applications; collaborate with teams to gather requirements and provide solutions</v>
+        <v>Master’s degree in GIS or related field with 3-5 years of GIS analysis experience; proficiency in ArcGIS Enterprise and Python (ArcPy) | Manage and analyze geospatial data, create and maintain spatial databases, conduct geospatial analysis, and provide user training</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2026-01-03T13:46:20.396Z</v>
+        <v>2026-01-04T10:30:01.863Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1566,7 +1557,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126919999</v>
+        <v>https://www.naukri.com/job-listings-it-recruiter-delivede-tamilnadu-chennai-1-to-3-years-030126010305</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1578,69 +1569,66 @@
         <v>Yes</v>
       </c>
       <c r="H15" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I15" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K15" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L15" t="str">
         <v>Skipped</v>
       </c>
       <c r="M15" t="str">
-        <v>Application Developer</v>
+        <v>It Recruiter</v>
       </c>
       <c r="N15" t="str">
-        <v>Accenture</v>
+        <v>Delivede Pvt Ltd</v>
       </c>
       <c r="O15" t="str">
-        <v>2 - 5 years</v>
+        <v>1 - 3 years</v>
       </c>
       <c r="P15" t="str">
-        <v>Not Disclosed</v>
+        <v>2.25-3.25 Lacs P.A.</v>
       </c>
       <c r="Q15" t="str">
         <v>Chennai</v>
       </c>
       <c r="R15" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S15" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T15" t="str">
-        <v>Less than 10</v>
+        <v>50</v>
       </c>
       <c r="U15" t="str">
-        <v>html, events, asynchronous apex, javascript, node, ATCI-5153530-S1900749, css, web services, hibernate, jquery, microservices, sql, spring, git, java, asp.net, j2ee, mongodb, c#, rest, version control, application development, spring boot, angular, node.js, javascript frameworks, angularjs</v>
+        <v>Java Developer, iOS Developer, Android Developer, Full Stack Developer, Backend Developer, Frontend Developer, Content Writer, HTML, SEO</v>
       </c>
       <c r="V15" t="str">
-        <v>Full Stack Developer</v>
+        <v>IT Recruiter</v>
       </c>
       <c r="W15" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Recruitment / Staffing</v>
       </c>
       <c r="X15" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y15" t="str">
-        <v>Software Development</v>
-      </c>
-      <c r="Z15" t="str">
-        <v>3.7</v>
+        <v>Recruitment &amp; Talent Acquisition</v>
       </c>
       <c r="AA15" t="str">
-        <v>Minimum 3 years experience in Node.js and 15 years full-time education | Design, build, and configure applications; collaborate with teams to gather requirements and provide solutions</v>
+        <v>Male candidate with skills in Java, Android, iOS, Full Stack, QA, .Net, SAP, PHP, UI/UX, Frontend, Backend, Content Writing, or Graphics Design | Handle end-to-end recruitment, schedule interviews, screen resumes, and report to Team Lead</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2026-01-03T13:46:25.055Z</v>
+        <v>2026-01-04T10:30:06.982Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1649,7 +1637,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-020126911772</v>
+        <v>https://www.naukri.com/job-listings-sr-associate-service-desk-agent-technical-support-apply-now-outpace-consulting-services-indore-chennai-mumbai-all-areas-1-to-5-years-231225036286</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1670,57 +1658,57 @@
         <v>Poor Match</v>
       </c>
       <c r="K16" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L16" t="str">
         <v>Skipped</v>
       </c>
       <c r="M16" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Sr Associate : Service Desk Agent : Technical Support : Apply Now</v>
       </c>
       <c r="N16" t="str">
-        <v>Accenture</v>
+        <v>Leading ITES Company</v>
       </c>
       <c r="O16" t="str">
-        <v>2 - 5 years</v>
+        <v>1 - 5 years</v>
       </c>
       <c r="P16" t="str">
-        <v>Not Disclosed</v>
+        <v>3-6 Lacs P.A.</v>
       </c>
       <c r="Q16" t="str">
-        <v>Pune</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R16" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S16" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T16" t="str">
+        <v>100+</v>
       </c>
       <c r="U16" t="str">
-        <v>software engineer, cloud services, software development, full stack development, strategic planning, web development frameworks, application development, cloud, database management, java, full stack, software solutions, web development, agile</v>
+        <v>Service Desk, Accenture, Active Directory, Google Workspace, Infy, Shivami, Hyperscaler, CTS, Econz, Firstsource, IT Support, Troubleshooting, Infosys, Ticketing Tools, Technical Support, Microsoft, Concentrix, AWS, Taskus, Searc, ITIL, 66 Degree, GCP, Sutherland, Teleperformance, Amazon, Hexaware</v>
       </c>
       <c r="V16" t="str">
-        <v>Back End Developer</v>
+        <v>IT Support - Other</v>
       </c>
       <c r="W16" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>BPM / BPO</v>
       </c>
       <c r="X16" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y16" t="str">
-        <v>Software Development</v>
-      </c>
-      <c r="Z16" t="str">
-        <v>3.7</v>
+        <v>IT Support</v>
       </c>
       <c r="AA16" t="str">
-        <v>Minimum 5 years experience in Java Full Stack Development with strong web development skills | Develop custom software solutions, collaborate with teams, mentor junior members</v>
+        <v>Graduate with 6+ months in Core Tech Support, experience in AWS/Azure/Google Cloud | Provide technical support via chat, troubleshoot issues, handle service requests, document resolutions</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2026-01-03T13:46:29.762Z</v>
+        <v>2026-01-04T10:30:11.842Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1729,13 +1717,13 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126920000</v>
+        <v>https://www.naukri.com/job-listings-servicenow-develope-vulnerability-secops-longterm-contact-pan-india-cloudxtreme-kolkata-bengaluru-delhi-ncr-3-to-8-years-171225015416</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
       </c>
       <c r="F17" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G17" t="str">
         <v>Yes</v>
@@ -1744,46 +1732,46 @@
         <v>Yes</v>
       </c>
       <c r="I17" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J17" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K17" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L17" t="str">
         <v>Skipped</v>
       </c>
       <c r="M17" t="str">
-        <v>Application Developer</v>
+        <v>ServiceNow develope &amp; Vulnerability (SecOps)longterm contact pan india</v>
       </c>
       <c r="N17" t="str">
-        <v>Accenture</v>
+        <v>Cloudxtreme</v>
       </c>
       <c r="O17" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P17" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q17" t="str">
-        <v>Chennai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R17" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S17" t="str">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="T17" t="str">
-        <v>Less than 10</v>
+        <v>22</v>
       </c>
       <c r="U17" t="str">
-        <v>html, events, asynchronous apex, javascript, node, css, web services, hibernate, jquery, microservices, sql, spring, git, java, asp.net, j2ee, mongodb, c#, rest, version control, ATCI-5153536-S1900738, application development, spring boot, angular, node.js, javascript frameworks, angularjs</v>
+        <v>ServiceNow, Vulnerability, MID Server, JavaScript and Glide APIs, REST and SOAP APIs, Flow Designer, Vulnerability Lifecycle Management, IntegrationHub, Qualys Rapid7 Tenable, CVE CWE, SecOps, Security Operations</v>
       </c>
       <c r="V17" t="str">
-        <v>Full Stack Developer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W17" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1795,15 +1783,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z17" t="str">
-        <v>3.7</v>
+        <v>3.0</v>
       </c>
       <c r="AA17" t="str">
-        <v>Minimum 3 years of experience in Node.js and 15 years of full-time education | Design, build, and configure applications; collaborate with teams to gather requirements and provide solutions</v>
+        <v>3-8 years of experience in ServiceNow Security Operations with a focus on Vulnerability Response; hands-on experience with tools like Qualys, Rapid7, and Tenable | Implement and optimize ServiceNow SecOps Vulnerability Response module; design and maintain integrations with security tools; manage workflows and vulnerability lifecycle</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2026-01-03T13:46:34.539Z</v>
+        <v>2026-01-04T10:30:16.666Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1812,7 +1800,7 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126919982</v>
+        <v>https://www.naukri.com/job-listings-power-bi-developer-go-digital-technology-consulting-mumbai-all-areas-3-to-6-years-030126015623</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
@@ -1821,52 +1809,52 @@
         <v>Yes</v>
       </c>
       <c r="G18" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H18" t="str">
         <v>Yes</v>
       </c>
       <c r="I18" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J18" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K18" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L18" t="str">
         <v>Skipped</v>
       </c>
       <c r="M18" t="str">
-        <v>Application Developer</v>
+        <v>Power Bi Developer</v>
       </c>
       <c r="N18" t="str">
-        <v>Accenture</v>
+        <v>Go Digital Technology Consulting</v>
       </c>
       <c r="O18" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P18" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q18" t="str">
-        <v>Chennai</v>
+        <v>Mumbai (All Areas)( Lower Parel )</v>
       </c>
       <c r="R18" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S18" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T18" t="str">
-        <v>12</v>
+        <v>100+</v>
       </c>
       <c r="U18" t="str">
-        <v>html, events, asynchronous apex, javascript, node, css, web services, hibernate, jquery, microservices, sql, spring, git, java, asp.net, j2ee, mongodb, c#, rest, version control, application development, spring boot, angular, node.js, ATCI-5153535-S1900997, javascript frameworks, angularjs</v>
+        <v>Power Query, SQL, Azure Data Factory, Dax, Data Modeling, Power Bi Service, Ci/Cd, Azure SQL, Data Warehousing Concepts, R, Agile, Scrum, Python</v>
       </c>
       <c r="V18" t="str">
-        <v>Full Stack Developer</v>
+        <v>Data Science &amp; Analytics - Other</v>
       </c>
       <c r="W18" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1875,18 +1863,18 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y18" t="str">
-        <v>Software Development</v>
+        <v>Data Science &amp; Analytics - Other</v>
       </c>
       <c r="Z18" t="str">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="AA18" t="str">
-        <v>Minimum 3 years experience in Node.js and 15 years full-time education | Design, build, and configure applications; collaborate with teams to gather requirements and provide solutions</v>
+        <v>Bachelor's degree in Computer Science or related field with 3+ years of Power BI development experience, strong skills in DAX and data modeling | Design, develop, and deploy interactive Power BI dashboards and reports; integrate with various data sources; optimize report performance</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2026-01-03T13:46:39.304Z</v>
+        <v>2026-01-04T10:30:21.506Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1895,81 +1883,81 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-application-developer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-020126919873</v>
+        <v>https://www.naukri.com/job-listings-api-automation-cloudxtreme-gandhinagar-3-to-6-years-031125017060</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
       </c>
       <c r="F19" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G19" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H19" t="str">
         <v>Yes</v>
       </c>
       <c r="I19" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J19" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K19" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L19" t="str">
         <v>Skipped</v>
       </c>
       <c r="M19" t="str">
-        <v>Application Developer</v>
+        <v>API Automation,</v>
       </c>
       <c r="N19" t="str">
-        <v>Accenture</v>
+        <v>Cloudxtreme</v>
       </c>
       <c r="O19" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P19" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q19" t="str">
-        <v>Chennai</v>
+        <v>Gandhinagar</v>
       </c>
       <c r="R19" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S19" t="str">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="T19" t="str">
-        <v>16</v>
+        <v>100+</v>
       </c>
       <c r="U19" t="str">
-        <v>redux, mobx, react.js, rest, javascript, css, web services, jsp, bootstrap, hibernate, jquery, apex, microservices, sql, spring, java, asp.net, json, html, mysql, c#, sql server, application development, spring boot, angular, node.js, troubleshooting, angularjs</v>
+        <v>Java, Rest Assured, Api Test Automation, Selenium, Cucumber, API Testing</v>
       </c>
       <c r="V19" t="str">
-        <v>Full Stack Developer</v>
+        <v>IT &amp; Information Security - Other</v>
       </c>
       <c r="W19" t="str">
         <v>IT Services &amp; Consulting</v>
       </c>
       <c r="X19" t="str">
-        <v>Full Time, Permanent</v>
+        <v>Full Time, Temporary/Contractual</v>
       </c>
       <c r="Y19" t="str">
-        <v>Software Development</v>
+        <v>IT &amp; Information Security - Other</v>
       </c>
       <c r="Z19" t="str">
-        <v>3.7</v>
+        <v>3.0</v>
       </c>
       <c r="AA19" t="str">
-        <v>Minimum 15 years of experience in React.js and strong front-end development skills | Design, build, and configure applications; collaborate with teams to gather requirements and optimize performance</v>
+        <v>3-6 years of IT experience with 2 years in API Rest Assured or automation tools; 3+ years in Java Selenium; hands-on experience in Cucumber and API testing | Set up Selenium environment, write and execute test cases, detect software flaws, and provide feedback on user requirements</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2026-01-03T13:46:44.100Z</v>
+        <v>2026-01-04T10:30:26.330Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1978,13 +1966,13 @@
         <v>19/20</v>
       </c>
       <c r="D20" t="str">
-        <v>https://www.naukri.com/job-listings-devloper-it-fullstack-ssc-welspun-transformation-services-limited-hyderabad-3-to-5-years-020126004987</v>
+        <v>https://www.naukri.com/job-listings-product-manager-instead-tax-india-private-limited-bengaluru-1-to-9-years-040126005162</v>
       </c>
       <c r="E20" t="str">
         <v>Yes</v>
       </c>
       <c r="F20" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G20" t="str">
         <v>Yes</v>
@@ -1993,10 +1981,10 @@
         <v>Yes</v>
       </c>
       <c r="I20" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J20" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K20" t="str">
         <v>Direct Apply</v>
@@ -2005,51 +1993,48 @@
         <v>Skipped</v>
       </c>
       <c r="M20" t="str">
-        <v>Devloper_IT_Fullstack_SSC</v>
+        <v>Product Manager</v>
       </c>
       <c r="N20" t="str">
-        <v>Welspun Transformation Services Limited</v>
+        <v>Instead</v>
       </c>
       <c r="O20" t="str">
-        <v>3 - 5 years</v>
+        <v>1 - 9 years</v>
       </c>
       <c r="P20" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q20" t="str">
-        <v>Hyderabad</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R20" t="str">
-        <v>1 day ago</v>
+        <v>Few hours ago</v>
       </c>
       <c r="S20" t="str">
         <v>100+</v>
       </c>
       <c r="U20" t="str">
-        <v>c#, rest, fullstack development, stack, css, bootstrap, hibernate, javascript, jquery, microservices, spring, react.js, angular, spring boot, node.js, java, full stack, json, html, mysql, front, angularjs, aws, mongodb</v>
+        <v>innovation, project management, software development, production, business analysis, facilitation, user stories, fintech, requirement gathering, operations, product management, saas, sprint planning, startup, quality assurance, cutting, agile, communication skills, agile methodology</v>
       </c>
       <c r="V20" t="str">
-        <v>Full Stack Developer</v>
+        <v>Product Manager - Pharma</v>
       </c>
       <c r="W20" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Internet</v>
       </c>
       <c r="X20" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y20" t="str">
-        <v>Software Development</v>
-      </c>
-      <c r="Z20" t="str">
-        <v>3.6</v>
+        <v>Product Management - Other</v>
       </c>
       <c r="AA20" t="str">
-        <v>Experience in full stack development with proficiency in C#, Java, and front-end technologies | Manage server-side logic and integrate front-end elements into applications</v>
+        <v>Background in product management with hands-on experience | Facilitate and manage projects for the tax technology platform, coordinate between global teams, and gather customer feedback | Competitive compensation and benefits</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2026-01-03T13:47:20.965Z</v>
+        <v>2026-01-04T10:30:31.243Z</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2058,46 +2043,46 @@
         <v>20/20</v>
       </c>
       <c r="D21" t="str">
-        <v>https://www.naukri.com/job-listings-application-support-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-020126919808</v>
+        <v>https://www.naukri.com/job-listings-hiring-for-tourism-manager-africa-location-time-legend-it-and-hr-consulting-solutions-kenya-democratic-republic-of-the-congo-central-african-republic-1-to-5-years-030126017809</v>
       </c>
       <c r="E21" t="str">
         <v>Yes</v>
       </c>
       <c r="F21" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G21" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H21" t="str">
         <v>Yes</v>
       </c>
       <c r="I21" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J21" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K21" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L21" t="str">
         <v>Skipped</v>
       </c>
       <c r="M21" t="str">
-        <v>Application Support Engineer</v>
+        <v>Hiring For Tourism Manager @Africa location</v>
       </c>
       <c r="N21" t="str">
-        <v>Accenture</v>
+        <v>Time Legend It And Hr Consulting Solutions</v>
       </c>
       <c r="O21" t="str">
-        <v>3 - 8 years</v>
+        <v>1 - 5 years</v>
       </c>
       <c r="P21" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q21" t="str">
-        <v>Chennai</v>
+        <v>Kenya</v>
       </c>
       <c r="R21" t="str">
         <v>1 day ago</v>
@@ -2106,28 +2091,28 @@
         <v>1</v>
       </c>
       <c r="T21" t="str">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U21" t="str">
-        <v>java fullstack, microservices, java, rest, spring boot, css, web services, jsp, jdbc, hibernate, jquery, sql, plsql, spring, git, spring mvc, linux, j2ee, html, mysql, mongodb, oracle, javascript, sql server, nosql, angular, node.js, application support, angularjs</v>
+        <v>Itinerary, FIT, Tourism, Holiday Packages, GIT, Sales</v>
       </c>
       <c r="V21" t="str">
-        <v>Database Developer / Engineer</v>
+        <v>Other</v>
       </c>
       <c r="W21" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Travel &amp; Tourism</v>
       </c>
       <c r="X21" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y21" t="str">
-        <v>DBA / Data warehousing</v>
+        <v>Other</v>
       </c>
       <c r="Z21" t="str">
-        <v>3.7</v>
+        <v>3.3</v>
       </c>
       <c r="AA21" t="str">
-        <v>Minimum 3 years experience in Spring Boot and 15 years full-time education | Identify and solve issues in critical business systems, collaborate with teams, and enhance system performance</v>
+        <v>Experience in sales with strong analytical and problem-solving skills | Manage sales and operations of holiday packages, design itineraries, and foster client relationships | Paid leave, travel allowances, and accommodation provided</v>
       </c>
     </row>
   </sheetData>

</xml_diff>